<commit_message>
pd: added location concepts - closes #73
See https://github.com/w3c/dpv/issues/73#issuecomment-2067725526
for info on links to be added to external vocabularies for detailed
representation of location concepts
</commit_message>
<xml_diff>
--- a/code/vocab_csv/pd.xlsx
+++ b/code/vocab_csv/pd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="831">
   <si>
     <t>Term</t>
   </si>
@@ -1906,15 +1906,6 @@
     <t>Information about personal possessions.</t>
   </si>
   <si>
-    <t>PhysicalAddress</t>
-  </si>
-  <si>
-    <t>Physical Address</t>
-  </si>
-  <si>
-    <t>Information about physical address.</t>
-  </si>
-  <si>
     <t>PhysicalCharacteristic</t>
   </si>
   <si>
@@ -2111,15 +2102,6 @@
   </si>
   <si>
     <t>Information about retina and the retinal patterns.</t>
-  </si>
-  <si>
-    <t>RoomNumber</t>
-  </si>
-  <si>
-    <t>Room Number</t>
-  </si>
-  <si>
-    <t>Information about location expressed as Room number or similar numbering systems</t>
   </si>
   <si>
     <t>Salary</t>
@@ -2445,19 +2427,43 @@
     <t>Citizenship</t>
   </si>
   <si>
+    <t>Information about citizenship</t>
+  </si>
+  <si>
     <t>Residency</t>
   </si>
   <si>
+    <t>Information about residency e.g. which region or country a person is resident in</t>
+  </si>
+  <si>
+    <t>dpv:Location</t>
+  </si>
+  <si>
     <t>Domicile</t>
   </si>
   <si>
+    <t>Information about domicile status e.g. which region or country a person is domiciled in</t>
+  </si>
+  <si>
     <t>PlaceOfBirth</t>
   </si>
   <si>
+    <t>Place Of Birth</t>
+  </si>
+  <si>
+    <t>Information about place of birth</t>
+  </si>
+  <si>
     <t>CountryOfBirth</t>
   </si>
   <si>
-    <t>IdentityDocument</t>
+    <t>Country Of Birth</t>
+  </si>
+  <si>
+    <t>Information about country of birth</t>
+  </si>
+  <si>
+    <t>dpv:Country</t>
   </si>
   <si>
     <t>Special Categories</t>
@@ -2569,6 +2575,84 @@
   </si>
   <si>
     <t>pd:GroupMembership,dpv:SpecialCategoryPersonalData</t>
+  </si>
+  <si>
+    <t>PhysicalAddress</t>
+  </si>
+  <si>
+    <t>Physical Address</t>
+  </si>
+  <si>
+    <t>Information about physical address.</t>
+  </si>
+  <si>
+    <t>pd:Contact,pd:Location</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>Elmar Kiesling; Harshvardhan J. Pandit, Fajar Ekaputra, Beatriz Esteves</t>
+  </si>
+  <si>
+    <t>Information about country as a location</t>
+  </si>
+  <si>
+    <t>pd:PhysicalAddress</t>
+  </si>
+  <si>
+    <t>Beatriz Esteves</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Information about region as a location</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Information about city as a location</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Information about street as a location</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Information about postal code as a location</t>
+  </si>
+  <si>
+    <t>Locality</t>
+  </si>
+  <si>
+    <t>Information about locality e.g. city, village, town, portion of a city as a location</t>
+  </si>
+  <si>
+    <t>HouseNumber</t>
+  </si>
+  <si>
+    <t>House Number</t>
+  </si>
+  <si>
+    <t>Information about house or apartment number as a location</t>
+  </si>
+  <si>
+    <t>RoomNumber</t>
+  </si>
+  <si>
+    <t>Room Number</t>
+  </si>
+  <si>
+    <t>Information about location expressed as Room number or similar numbering systems</t>
   </si>
   <si>
     <t>dpv:SpecialCategoryPersonalData</t>
@@ -2581,7 +2665,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2712,12 +2796,6 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2795,7 +2873,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2966,7 +3044,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -20274,10 +20351,6 @@
       <c r="E105" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F105" s="12"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="12"/>
-      <c r="I105" s="12"/>
       <c r="J105" s="29" t="s">
         <v>162</v>
       </c>
@@ -20296,19 +20369,6 @@
       <c r="O105" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="P105" s="12"/>
-      <c r="Q105" s="12"/>
-      <c r="R105" s="12"/>
-      <c r="S105" s="12"/>
-      <c r="T105" s="12"/>
-      <c r="U105" s="12"/>
-      <c r="V105" s="12"/>
-      <c r="W105" s="12"/>
-      <c r="X105" s="12"/>
-      <c r="Y105" s="12"/>
-      <c r="Z105" s="12"/>
-      <c r="AA105" s="12"/>
-      <c r="AB105" s="12"/>
     </row>
     <row r="106">
       <c r="A106" s="10" t="s">
@@ -21556,65 +21616,15 @@
       <c r="AA130" s="12"/>
       <c r="AB130" s="12"/>
     </row>
-    <row r="131">
-      <c r="A131" s="10" t="s">
-        <v>587</v>
-      </c>
-      <c r="B131" s="25" t="s">
-        <v>588</v>
-      </c>
-      <c r="C131" s="10" t="s">
-        <v>589</v>
-      </c>
-      <c r="D131" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F131" s="12"/>
-      <c r="G131" s="12"/>
-      <c r="H131" s="12"/>
-      <c r="I131" s="12"/>
-      <c r="J131" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="K131" s="13">
-        <v>43620.0</v>
-      </c>
-      <c r="L131" s="12"/>
-      <c r="M131" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N131" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="O131" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="P131" s="12"/>
-      <c r="Q131" s="12"/>
-      <c r="R131" s="12"/>
-      <c r="S131" s="12"/>
-      <c r="T131" s="12"/>
-      <c r="U131" s="12"/>
-      <c r="V131" s="12"/>
-      <c r="W131" s="12"/>
-      <c r="X131" s="12"/>
-      <c r="Y131" s="12"/>
-      <c r="Z131" s="12"/>
-      <c r="AA131" s="12"/>
-      <c r="AB131" s="12"/>
-    </row>
     <row r="132">
       <c r="A132" s="10" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D132" s="10" t="s">
         <v>224</v>
@@ -21624,7 +21634,7 @@
       </c>
       <c r="F132" s="12"/>
       <c r="G132" s="12" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="H132" s="12"/>
       <c r="I132" s="12"/>
@@ -21660,13 +21670,13 @@
     </row>
     <row r="133">
       <c r="A133" s="10" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D133" s="10" t="s">
         <v>449</v>
@@ -21710,13 +21720,13 @@
     </row>
     <row r="134">
       <c r="A134" s="10" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>453</v>
@@ -21760,13 +21770,13 @@
     </row>
     <row r="135">
       <c r="A135" s="10" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>540</v>
@@ -21810,13 +21820,13 @@
     </row>
     <row r="136">
       <c r="A136" s="10" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C136" s="45" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D136" s="10" t="s">
         <v>192</v>
@@ -21860,13 +21870,13 @@
     </row>
     <row r="137">
       <c r="A137" s="10" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D137" s="10" t="s">
         <v>560</v>
@@ -21910,13 +21920,13 @@
     </row>
     <row r="138">
       <c r="A138" s="10" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D138" s="10" t="s">
         <v>213</v>
@@ -21926,7 +21936,7 @@
       </c>
       <c r="F138" s="12"/>
       <c r="G138" s="12" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="H138" s="12"/>
       <c r="I138" s="12"/>
@@ -21962,13 +21972,13 @@
     </row>
     <row r="139">
       <c r="A139" s="10" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B139" s="25" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D139" s="10" t="s">
         <v>236</v>
@@ -22012,13 +22022,13 @@
     </row>
     <row r="140">
       <c r="A140" s="10" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B140" s="25" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D140" s="10" t="s">
         <v>413</v>
@@ -22062,13 +22072,13 @@
     </row>
     <row r="141">
       <c r="A141" s="10" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D141" s="10" t="s">
         <v>426</v>
@@ -22112,13 +22122,13 @@
     </row>
     <row r="142">
       <c r="A142" s="10" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D142" s="10" t="s">
         <v>265</v>
@@ -22162,13 +22172,13 @@
     </row>
     <row r="143">
       <c r="A143" s="10" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D143" s="10" t="s">
         <v>355</v>
@@ -22212,13 +22222,13 @@
     </row>
     <row r="144">
       <c r="A144" s="10" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B144" s="25" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D144" s="10" t="s">
         <v>355</v>
@@ -22262,13 +22272,13 @@
     </row>
     <row r="145">
       <c r="A145" s="10" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D145" s="10" t="s">
         <v>355</v>
@@ -22312,16 +22322,16 @@
     </row>
     <row r="146">
       <c r="A146" s="10" t="s">
+        <v>625</v>
+      </c>
+      <c r="B146" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="C146" s="10" t="s">
+        <v>627</v>
+      </c>
+      <c r="D146" s="10" t="s">
         <v>628</v>
-      </c>
-      <c r="B146" s="11" t="s">
-        <v>629</v>
-      </c>
-      <c r="C146" s="10" t="s">
-        <v>630</v>
-      </c>
-      <c r="D146" s="10" t="s">
-        <v>631</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>52</v>
@@ -22331,12 +22341,16 @@
       <c r="H146" s="12"/>
       <c r="I146" s="12"/>
       <c r="J146" s="12"/>
-      <c r="K146" s="42"/>
+      <c r="K146" s="42">
+        <v>45402.0</v>
+      </c>
       <c r="L146" s="12"/>
       <c r="M146" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="N146" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="N146" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="O146" s="30"/>
       <c r="P146" s="12"/>
       <c r="Q146" s="12"/>
@@ -22354,16 +22368,16 @@
     </row>
     <row r="147">
       <c r="A147" s="10" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>52</v>
@@ -22373,12 +22387,16 @@
       <c r="H147" s="12"/>
       <c r="I147" s="12"/>
       <c r="J147" s="19"/>
-      <c r="K147" s="13"/>
+      <c r="K147" s="13">
+        <v>45402.0</v>
+      </c>
       <c r="L147" s="12"/>
       <c r="M147" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N147" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="N147" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="O147" s="10"/>
       <c r="P147" s="12"/>
       <c r="Q147" s="12"/>
@@ -22396,13 +22414,13 @@
     </row>
     <row r="148">
       <c r="A148" s="10" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D148" s="10" t="s">
         <v>265</v>
@@ -22446,16 +22464,16 @@
     </row>
     <row r="149">
       <c r="A149" s="10" t="s">
+        <v>635</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="D149" s="10" t="s">
         <v>638</v>
-      </c>
-      <c r="B149" s="11" t="s">
-        <v>639</v>
-      </c>
-      <c r="C149" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="D149" s="10" t="s">
-        <v>641</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>52</v>
@@ -22494,13 +22512,13 @@
     </row>
     <row r="150">
       <c r="A150" s="10" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D150" s="10" t="s">
         <v>280</v>
@@ -22510,7 +22528,7 @@
       </c>
       <c r="F150" s="10"/>
       <c r="G150" s="10" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H150" s="12"/>
       <c r="I150" s="12"/>
@@ -22546,13 +22564,13 @@
     </row>
     <row r="151">
       <c r="A151" s="10" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B151" s="25" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D151" s="10" t="s">
         <v>280</v>
@@ -22596,13 +22614,13 @@
     </row>
     <row r="152">
       <c r="A152" s="10" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B152" s="25" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D152" s="10" t="s">
         <v>355</v>
@@ -22646,13 +22664,13 @@
     </row>
     <row r="153">
       <c r="A153" s="10" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D153" s="10" t="s">
         <v>410</v>
@@ -22696,13 +22714,13 @@
     </row>
     <row r="154">
       <c r="A154" s="10" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D154" s="10" t="s">
         <v>210</v>
@@ -22744,13 +22762,13 @@
     </row>
     <row r="155">
       <c r="A155" s="10" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B155" s="25" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D155" s="10" t="s">
         <v>400</v>
@@ -22794,16 +22812,16 @@
     </row>
     <row r="156">
       <c r="A156" s="10" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B156" s="25" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="D156" s="10" t="s">
-        <v>232</v>
+        <v>355</v>
       </c>
       <c r="E156" s="9" t="s">
         <v>52</v>
@@ -22844,16 +22862,16 @@
     </row>
     <row r="157">
       <c r="A157" s="10" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D157" s="10" t="s">
-        <v>355</v>
+        <v>280</v>
       </c>
       <c r="E157" s="9" t="s">
         <v>52</v>
@@ -22894,16 +22912,16 @@
     </row>
     <row r="158">
       <c r="A158" s="10" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D158" s="10" t="s">
-        <v>280</v>
+        <v>355</v>
       </c>
       <c r="E158" s="9" t="s">
         <v>52</v>
@@ -22944,16 +22962,16 @@
     </row>
     <row r="159">
       <c r="A159" s="10" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B159" s="25" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>355</v>
+        <v>560</v>
       </c>
       <c r="E159" s="9" t="s">
         <v>52</v>
@@ -22994,16 +23012,16 @@
     </row>
     <row r="160">
       <c r="A160" s="10" t="s">
-        <v>665</v>
-      </c>
-      <c r="B160" s="25" t="s">
-        <v>666</v>
+        <v>662</v>
+      </c>
+      <c r="B160" s="11" t="s">
+        <v>663</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D160" s="10" t="s">
-        <v>560</v>
+        <v>210</v>
       </c>
       <c r="E160" s="9" t="s">
         <v>52</v>
@@ -23012,21 +23030,21 @@
       <c r="G160" s="12"/>
       <c r="H160" s="12"/>
       <c r="I160" s="12"/>
-      <c r="J160" s="29" t="s">
-        <v>162</v>
+      <c r="J160" s="16" t="s">
+        <v>665</v>
       </c>
       <c r="K160" s="13">
-        <v>43620.0</v>
+        <v>43795.0</v>
       </c>
       <c r="L160" s="12"/>
       <c r="M160" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N160" s="10" t="s">
-        <v>96</v>
+        <v>666</v>
       </c>
       <c r="O160" s="14" t="s">
-        <v>163</v>
+        <v>667</v>
       </c>
       <c r="P160" s="12"/>
       <c r="Q160" s="12"/>
@@ -23046,14 +23064,14 @@
       <c r="A161" s="10" t="s">
         <v>668</v>
       </c>
-      <c r="B161" s="11" t="s">
+      <c r="B161" s="25" t="s">
         <v>669</v>
       </c>
       <c r="C161" s="10" t="s">
         <v>670</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>210</v>
+        <v>426</v>
       </c>
       <c r="E161" s="9" t="s">
         <v>52</v>
@@ -23062,21 +23080,21 @@
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
       <c r="I161" s="12"/>
-      <c r="J161" s="16" t="s">
-        <v>671</v>
+      <c r="J161" s="29" t="s">
+        <v>162</v>
       </c>
       <c r="K161" s="13">
-        <v>43795.0</v>
+        <v>43620.0</v>
       </c>
       <c r="L161" s="12"/>
       <c r="M161" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N161" s="10" t="s">
-        <v>672</v>
+        <v>96</v>
       </c>
       <c r="O161" s="14" t="s">
-        <v>673</v>
+        <v>163</v>
       </c>
       <c r="P161" s="12"/>
       <c r="Q161" s="12"/>
@@ -23094,13 +23112,13 @@
     </row>
     <row r="162">
       <c r="A162" s="10" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="B162" s="25" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D162" s="10" t="s">
         <v>426</v>
@@ -23144,16 +23162,16 @@
     </row>
     <row r="163">
       <c r="A163" s="10" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>678</v>
-      </c>
-      <c r="C163" s="10" t="s">
-        <v>679</v>
+        <v>674</v>
+      </c>
+      <c r="C163" s="46" t="s">
+        <v>675</v>
       </c>
       <c r="D163" s="10" t="s">
-        <v>426</v>
+        <v>361</v>
       </c>
       <c r="E163" s="9" t="s">
         <v>52</v>
@@ -23194,16 +23212,16 @@
     </row>
     <row r="164">
       <c r="A164" s="10" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="B164" s="25" t="s">
-        <v>680</v>
-      </c>
-      <c r="C164" s="46" t="s">
-        <v>681</v>
+        <v>677</v>
+      </c>
+      <c r="C164" s="10" t="s">
+        <v>678</v>
       </c>
       <c r="D164" s="10" t="s">
-        <v>361</v>
+        <v>192</v>
       </c>
       <c r="E164" s="9" t="s">
         <v>52</v>
@@ -23244,22 +23262,24 @@
     </row>
     <row r="165">
       <c r="A165" s="10" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>683</v>
-      </c>
-      <c r="C165" s="10" t="s">
-        <v>684</v>
+        <v>680</v>
+      </c>
+      <c r="C165" s="46" t="s">
+        <v>681</v>
       </c>
       <c r="D165" s="10" t="s">
-        <v>192</v>
+        <v>391</v>
       </c>
       <c r="E165" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F165" s="12"/>
-      <c r="G165" s="12"/>
+      <c r="G165" s="12" t="s">
+        <v>682</v>
+      </c>
       <c r="H165" s="12"/>
       <c r="I165" s="12"/>
       <c r="J165" s="29" t="s">
@@ -23294,13 +23314,13 @@
     </row>
     <row r="166">
       <c r="A166" s="10" t="s">
+        <v>683</v>
+      </c>
+      <c r="B166" s="11" t="s">
+        <v>684</v>
+      </c>
+      <c r="C166" s="10" t="s">
         <v>685</v>
-      </c>
-      <c r="B166" s="25" t="s">
-        <v>686</v>
-      </c>
-      <c r="C166" s="46" t="s">
-        <v>687</v>
       </c>
       <c r="D166" s="10" t="s">
         <v>391</v>
@@ -23309,26 +23329,22 @@
         <v>52</v>
       </c>
       <c r="F166" s="12"/>
-      <c r="G166" s="12" t="s">
-        <v>688</v>
-      </c>
+      <c r="G166" s="12"/>
       <c r="H166" s="12"/>
       <c r="I166" s="12"/>
-      <c r="J166" s="29" t="s">
-        <v>162</v>
-      </c>
+      <c r="J166" s="12"/>
       <c r="K166" s="13">
-        <v>43620.0</v>
+        <v>44727.0</v>
       </c>
       <c r="L166" s="12"/>
-      <c r="M166" s="10" t="s">
+      <c r="M166" s="30" t="s">
         <v>19</v>
       </c>
       <c r="N166" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="O166" s="14" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="P166" s="12"/>
       <c r="Q166" s="12"/>
@@ -23346,16 +23362,16 @@
     </row>
     <row r="167">
       <c r="A167" s="10" t="s">
-        <v>689</v>
-      </c>
-      <c r="B167" s="11" t="s">
-        <v>690</v>
+        <v>686</v>
+      </c>
+      <c r="B167" s="25" t="s">
+        <v>687</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D167" s="10" t="s">
-        <v>391</v>
+        <v>265</v>
       </c>
       <c r="E167" s="9" t="s">
         <v>52</v>
@@ -23364,19 +23380,21 @@
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
       <c r="I167" s="12"/>
-      <c r="J167" s="12"/>
+      <c r="J167" s="29" t="s">
+        <v>162</v>
+      </c>
       <c r="K167" s="13">
-        <v>44727.0</v>
+        <v>43620.0</v>
       </c>
       <c r="L167" s="12"/>
-      <c r="M167" s="30" t="s">
+      <c r="M167" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N167" s="10" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="O167" s="14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="P167" s="12"/>
       <c r="Q167" s="12"/>
@@ -23394,16 +23412,16 @@
     </row>
     <row r="168">
       <c r="A168" s="10" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="B168" s="25" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E168" s="9" t="s">
         <v>52</v>
@@ -23444,16 +23462,16 @@
     </row>
     <row r="169">
       <c r="A169" s="10" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="D169" s="10" t="s">
-        <v>262</v>
+        <v>192</v>
       </c>
       <c r="E169" s="9" t="s">
         <v>52</v>
@@ -23494,16 +23512,16 @@
     </row>
     <row r="170">
       <c r="A170" s="10" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D170" s="10" t="s">
-        <v>192</v>
+        <v>280</v>
       </c>
       <c r="E170" s="9" t="s">
         <v>52</v>
@@ -23544,16 +23562,16 @@
     </row>
     <row r="171">
       <c r="A171" s="10" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D171" s="10" t="s">
-        <v>280</v>
+        <v>380</v>
       </c>
       <c r="E171" s="9" t="s">
         <v>52</v>
@@ -23569,7 +23587,7 @@
         <v>43620.0</v>
       </c>
       <c r="L171" s="12"/>
-      <c r="M171" s="10" t="s">
+      <c r="M171" s="21" t="s">
         <v>19</v>
       </c>
       <c r="N171" s="10" t="s">
@@ -23593,17 +23611,17 @@
       <c r="AB171" s="12"/>
     </row>
     <row r="172">
-      <c r="A172" s="10" t="s">
-        <v>702</v>
-      </c>
-      <c r="B172" s="25" t="s">
-        <v>703</v>
-      </c>
-      <c r="C172" s="10" t="s">
-        <v>704</v>
+      <c r="A172" s="46" t="s">
+        <v>699</v>
+      </c>
+      <c r="B172" s="57" t="s">
+        <v>699</v>
+      </c>
+      <c r="C172" s="45" t="s">
+        <v>700</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>380</v>
+        <v>701</v>
       </c>
       <c r="E172" s="9" t="s">
         <v>52</v>
@@ -23619,7 +23637,7 @@
         <v>43620.0</v>
       </c>
       <c r="L172" s="12"/>
-      <c r="M172" s="21" t="s">
+      <c r="M172" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N172" s="10" t="s">
@@ -23643,17 +23661,17 @@
       <c r="AB172" s="12"/>
     </row>
     <row r="173">
-      <c r="A173" s="46" t="s">
-        <v>705</v>
-      </c>
-      <c r="B173" s="57" t="s">
-        <v>705</v>
-      </c>
-      <c r="C173" s="45" t="s">
-        <v>706</v>
+      <c r="A173" s="10" t="s">
+        <v>702</v>
+      </c>
+      <c r="B173" s="23" t="s">
+        <v>702</v>
+      </c>
+      <c r="C173" s="10" t="s">
+        <v>703</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>707</v>
+        <v>280</v>
       </c>
       <c r="E173" s="9" t="s">
         <v>52</v>
@@ -23694,16 +23712,16 @@
     </row>
     <row r="174">
       <c r="A174" s="10" t="s">
-        <v>708</v>
-      </c>
-      <c r="B174" s="23" t="s">
-        <v>708</v>
+        <v>704</v>
+      </c>
+      <c r="B174" s="25" t="s">
+        <v>704</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>280</v>
+        <v>430</v>
       </c>
       <c r="E174" s="9" t="s">
         <v>52</v>
@@ -23744,16 +23762,16 @@
     </row>
     <row r="175">
       <c r="A175" s="10" t="s">
-        <v>710</v>
-      </c>
-      <c r="B175" s="25" t="s">
-        <v>710</v>
+        <v>706</v>
+      </c>
+      <c r="B175" s="11" t="s">
+        <v>707</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>430</v>
+        <v>232</v>
       </c>
       <c r="E175" s="9" t="s">
         <v>52</v>
@@ -23762,21 +23780,19 @@
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
       <c r="I175" s="12"/>
-      <c r="J175" s="29" t="s">
-        <v>162</v>
-      </c>
+      <c r="J175" s="19"/>
       <c r="K175" s="13">
-        <v>43620.0</v>
+        <v>44671.0</v>
       </c>
       <c r="L175" s="12"/>
       <c r="M175" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N175" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="O175" s="14" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="P175" s="12"/>
       <c r="Q175" s="12"/>
@@ -23794,16 +23810,16 @@
     </row>
     <row r="176">
       <c r="A176" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="B176" s="11" t="s">
+        <v>710</v>
+      </c>
+      <c r="C176" s="10" t="s">
+        <v>711</v>
+      </c>
+      <c r="D176" s="10" t="s">
         <v>712</v>
-      </c>
-      <c r="B176" s="11" t="s">
-        <v>713</v>
-      </c>
-      <c r="C176" s="10" t="s">
-        <v>714</v>
-      </c>
-      <c r="D176" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="E176" s="9" t="s">
         <v>52</v>
@@ -23812,19 +23828,21 @@
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
       <c r="I176" s="12"/>
-      <c r="J176" s="19"/>
+      <c r="J176" s="16" t="s">
+        <v>713</v>
+      </c>
       <c r="K176" s="13">
-        <v>44671.0</v>
+        <v>43795.0</v>
       </c>
       <c r="L176" s="12"/>
       <c r="M176" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N176" s="10" t="s">
-        <v>20</v>
+        <v>666</v>
       </c>
       <c r="O176" s="14" t="s">
-        <v>197</v>
+        <v>667</v>
       </c>
       <c r="P176" s="12"/>
       <c r="Q176" s="12"/>
@@ -23842,39 +23860,41 @@
     </row>
     <row r="177">
       <c r="A177" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="B177" s="25" t="s">
+        <v>714</v>
+      </c>
+      <c r="C177" s="10" t="s">
         <v>715</v>
       </c>
-      <c r="B177" s="11" t="s">
-        <v>716</v>
-      </c>
-      <c r="C177" s="10" t="s">
-        <v>717</v>
-      </c>
       <c r="D177" s="10" t="s">
-        <v>718</v>
+        <v>540</v>
       </c>
       <c r="E177" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F177" s="12"/>
-      <c r="G177" s="12"/>
+      <c r="F177" s="10"/>
+      <c r="G177" s="10" t="s">
+        <v>716</v>
+      </c>
       <c r="H177" s="12"/>
       <c r="I177" s="12"/>
-      <c r="J177" s="16" t="s">
-        <v>719</v>
+      <c r="J177" s="29" t="s">
+        <v>162</v>
       </c>
       <c r="K177" s="13">
-        <v>43795.0</v>
+        <v>43620.0</v>
       </c>
       <c r="L177" s="12"/>
       <c r="M177" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N177" s="10" t="s">
-        <v>672</v>
+        <v>96</v>
       </c>
       <c r="O177" s="14" t="s">
-        <v>673</v>
+        <v>163</v>
       </c>
       <c r="P177" s="12"/>
       <c r="Q177" s="12"/>
@@ -23892,116 +23912,114 @@
     </row>
     <row r="178">
       <c r="A178" s="10" t="s">
-        <v>720</v>
-      </c>
-      <c r="B178" s="25" t="s">
-        <v>720</v>
-      </c>
-      <c r="C178" s="10" t="s">
-        <v>721</v>
-      </c>
-      <c r="D178" s="10" t="s">
-        <v>540</v>
+        <v>717</v>
+      </c>
+      <c r="B178" s="30" t="s">
+        <v>718</v>
+      </c>
+      <c r="C178" s="58" t="s">
+        <v>719</v>
+      </c>
+      <c r="D178" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="E178" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F178" s="10"/>
-      <c r="G178" s="10" t="s">
-        <v>722</v>
-      </c>
-      <c r="H178" s="12"/>
-      <c r="I178" s="12"/>
-      <c r="J178" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="K178" s="13">
-        <v>43620.0</v>
-      </c>
-      <c r="L178" s="12"/>
-      <c r="M178" s="10" t="s">
+      <c r="F178" s="59"/>
+      <c r="G178" s="59"/>
+      <c r="H178" s="59"/>
+      <c r="I178" s="59"/>
+      <c r="J178" s="30"/>
+      <c r="K178" s="42">
+        <v>44727.0</v>
+      </c>
+      <c r="L178" s="42"/>
+      <c r="M178" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="N178" s="10" t="s">
-        <v>96</v>
+      <c r="N178" s="30" t="s">
+        <v>106</v>
       </c>
       <c r="O178" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="P178" s="12"/>
-      <c r="Q178" s="12"/>
-      <c r="R178" s="12"/>
-      <c r="S178" s="12"/>
-      <c r="T178" s="12"/>
-      <c r="U178" s="12"/>
-      <c r="V178" s="12"/>
-      <c r="W178" s="12"/>
-      <c r="X178" s="12"/>
-      <c r="Y178" s="12"/>
-      <c r="Z178" s="12"/>
-      <c r="AA178" s="12"/>
-      <c r="AB178" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="P178" s="59"/>
+      <c r="Q178" s="59"/>
+      <c r="R178" s="59"/>
+      <c r="S178" s="59"/>
+      <c r="T178" s="59"/>
+      <c r="U178" s="59"/>
+      <c r="V178" s="59"/>
+      <c r="W178" s="59"/>
+      <c r="X178" s="59"/>
+      <c r="Y178" s="59"/>
+      <c r="Z178" s="59"/>
+      <c r="AA178" s="59"/>
+      <c r="AB178" s="59"/>
     </row>
     <row r="179">
       <c r="A179" s="10" t="s">
-        <v>723</v>
-      </c>
-      <c r="B179" s="30" t="s">
-        <v>724</v>
-      </c>
-      <c r="C179" s="58" t="s">
-        <v>725</v>
-      </c>
-      <c r="D179" s="30" t="s">
-        <v>274</v>
+        <v>720</v>
+      </c>
+      <c r="B179" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="C179" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="D179" s="10" t="s">
+        <v>540</v>
       </c>
       <c r="E179" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F179" s="59"/>
-      <c r="G179" s="59"/>
-      <c r="H179" s="59"/>
-      <c r="I179" s="59"/>
-      <c r="J179" s="30"/>
-      <c r="K179" s="42">
-        <v>44727.0</v>
-      </c>
-      <c r="L179" s="42"/>
-      <c r="M179" s="30" t="s">
+      <c r="F179" s="12"/>
+      <c r="G179" s="12"/>
+      <c r="H179" s="12"/>
+      <c r="I179" s="12"/>
+      <c r="J179" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K179" s="13">
+        <v>43620.0</v>
+      </c>
+      <c r="L179" s="12"/>
+      <c r="M179" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N179" s="30" t="s">
-        <v>106</v>
+      <c r="N179" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="O179" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="P179" s="59"/>
-      <c r="Q179" s="59"/>
-      <c r="R179" s="59"/>
-      <c r="S179" s="59"/>
-      <c r="T179" s="59"/>
-      <c r="U179" s="59"/>
-      <c r="V179" s="59"/>
-      <c r="W179" s="59"/>
-      <c r="X179" s="59"/>
-      <c r="Y179" s="59"/>
-      <c r="Z179" s="59"/>
-      <c r="AA179" s="59"/>
-      <c r="AB179" s="59"/>
+        <v>163</v>
+      </c>
+      <c r="P179" s="12"/>
+      <c r="Q179" s="12"/>
+      <c r="R179" s="12"/>
+      <c r="S179" s="12"/>
+      <c r="T179" s="12"/>
+      <c r="U179" s="12"/>
+      <c r="V179" s="12"/>
+      <c r="W179" s="12"/>
+      <c r="X179" s="12"/>
+      <c r="Y179" s="12"/>
+      <c r="Z179" s="12"/>
+      <c r="AA179" s="12"/>
+      <c r="AB179" s="12"/>
     </row>
     <row r="180">
       <c r="A180" s="10" t="s">
-        <v>726</v>
-      </c>
-      <c r="B180" s="25" t="s">
-        <v>726</v>
+        <v>722</v>
+      </c>
+      <c r="B180" s="11" t="s">
+        <v>723</v>
       </c>
       <c r="C180" s="10" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>540</v>
+        <v>725</v>
       </c>
       <c r="E180" s="9" t="s">
         <v>52</v>
@@ -24010,21 +24028,19 @@
       <c r="G180" s="12"/>
       <c r="H180" s="12"/>
       <c r="I180" s="12"/>
-      <c r="J180" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="K180" s="13">
-        <v>43620.0</v>
+      <c r="J180" s="12"/>
+      <c r="K180" s="42">
+        <v>44727.0</v>
       </c>
       <c r="L180" s="12"/>
-      <c r="M180" s="10" t="s">
+      <c r="M180" s="30" t="s">
         <v>19</v>
       </c>
       <c r="N180" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="O180" s="14" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="P180" s="12"/>
       <c r="Q180" s="12"/>
@@ -24042,16 +24058,16 @@
     </row>
     <row r="181">
       <c r="A181" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="B181" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="C181" s="10" t="s">
         <v>728</v>
       </c>
-      <c r="B181" s="11" t="s">
-        <v>729</v>
-      </c>
-      <c r="C181" s="10" t="s">
-        <v>730</v>
-      </c>
       <c r="D181" s="10" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="E181" s="9" t="s">
         <v>52</v>
@@ -24061,7 +24077,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="12"/>
       <c r="J181" s="12"/>
-      <c r="K181" s="42">
+      <c r="K181" s="13">
         <v>44727.0</v>
       </c>
       <c r="L181" s="12"/>
@@ -24090,16 +24106,16 @@
     </row>
     <row r="182">
       <c r="A182" s="10" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>731</v>
+        <v>224</v>
       </c>
       <c r="E182" s="9" t="s">
         <v>52</v>
@@ -24138,16 +24154,16 @@
     </row>
     <row r="183">
       <c r="A183" s="10" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>224</v>
+        <v>734</v>
       </c>
       <c r="E183" s="9" t="s">
         <v>52</v>
@@ -24186,16 +24202,16 @@
     </row>
     <row r="184">
       <c r="A184" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="B184" s="11" t="s">
+        <v>736</v>
+      </c>
+      <c r="C184" s="10" t="s">
         <v>737</v>
       </c>
-      <c r="B184" s="11" t="s">
+      <c r="D184" s="10" t="s">
         <v>738</v>
-      </c>
-      <c r="C184" s="10" t="s">
-        <v>739</v>
-      </c>
-      <c r="D184" s="10" t="s">
-        <v>740</v>
       </c>
       <c r="E184" s="9" t="s">
         <v>52</v>
@@ -24205,7 +24221,7 @@
       <c r="H184" s="12"/>
       <c r="I184" s="12"/>
       <c r="J184" s="12"/>
-      <c r="K184" s="13">
+      <c r="K184" s="42">
         <v>44727.0</v>
       </c>
       <c r="L184" s="12"/>
@@ -24234,16 +24250,16 @@
     </row>
     <row r="185">
       <c r="A185" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="B185" s="25" t="s">
+        <v>740</v>
+      </c>
+      <c r="C185" s="46" t="s">
         <v>741</v>
       </c>
-      <c r="B185" s="11" t="s">
-        <v>742</v>
-      </c>
-      <c r="C185" s="10" t="s">
-        <v>743</v>
-      </c>
       <c r="D185" s="10" t="s">
-        <v>744</v>
+        <v>391</v>
       </c>
       <c r="E185" s="9" t="s">
         <v>52</v>
@@ -24251,20 +24267,22 @@
       <c r="F185" s="12"/>
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
-      <c r="I185" s="12"/>
-      <c r="J185" s="12"/>
-      <c r="K185" s="42">
-        <v>44727.0</v>
+      <c r="I185" s="28"/>
+      <c r="J185" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K185" s="13">
+        <v>43620.0</v>
       </c>
       <c r="L185" s="12"/>
-      <c r="M185" s="30" t="s">
+      <c r="M185" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N185" s="10" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="O185" s="14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="P185" s="12"/>
       <c r="Q185" s="12"/>
@@ -24282,13 +24300,13 @@
     </row>
     <row r="186">
       <c r="A186" s="10" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="B186" s="25" t="s">
-        <v>746</v>
-      </c>
-      <c r="C186" s="46" t="s">
-        <v>747</v>
+        <v>743</v>
+      </c>
+      <c r="C186" s="10" t="s">
+        <v>744</v>
       </c>
       <c r="D186" s="10" t="s">
         <v>391</v>
@@ -24299,7 +24317,7 @@
       <c r="F186" s="12"/>
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
-      <c r="I186" s="28"/>
+      <c r="I186" s="12"/>
       <c r="J186" s="29" t="s">
         <v>162</v>
       </c>
@@ -24332,16 +24350,16 @@
     </row>
     <row r="187">
       <c r="A187" s="10" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="B187" s="25" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>391</v>
+        <v>192</v>
       </c>
       <c r="E187" s="9" t="s">
         <v>52</v>
@@ -24382,16 +24400,16 @@
     </row>
     <row r="188">
       <c r="A188" s="10" t="s">
-        <v>751</v>
-      </c>
-      <c r="B188" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
+      </c>
+      <c r="B188" s="11" t="s">
+        <v>748</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>192</v>
+        <v>355</v>
       </c>
       <c r="E188" s="9" t="s">
         <v>52</v>
@@ -24400,21 +24418,19 @@
       <c r="G188" s="12"/>
       <c r="H188" s="12"/>
       <c r="I188" s="12"/>
-      <c r="J188" s="29" t="s">
-        <v>162</v>
-      </c>
+      <c r="J188" s="12"/>
       <c r="K188" s="13">
-        <v>43620.0</v>
+        <v>44727.0</v>
       </c>
       <c r="L188" s="12"/>
-      <c r="M188" s="10" t="s">
+      <c r="M188" s="30" t="s">
         <v>19</v>
       </c>
       <c r="N188" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="O188" s="14" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="P188" s="12"/>
       <c r="Q188" s="12"/>
@@ -24432,13 +24448,13 @@
     </row>
     <row r="189">
       <c r="A189" s="10" t="s">
-        <v>753</v>
-      </c>
-      <c r="B189" s="11" t="s">
-        <v>754</v>
+        <v>750</v>
+      </c>
+      <c r="B189" s="25" t="s">
+        <v>751</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="D189" s="10" t="s">
         <v>355</v>
@@ -24450,19 +24466,21 @@
       <c r="G189" s="12"/>
       <c r="H189" s="12"/>
       <c r="I189" s="12"/>
-      <c r="J189" s="12"/>
+      <c r="J189" s="29" t="s">
+        <v>162</v>
+      </c>
       <c r="K189" s="13">
-        <v>44727.0</v>
+        <v>43620.0</v>
       </c>
       <c r="L189" s="12"/>
-      <c r="M189" s="30" t="s">
+      <c r="M189" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N189" s="10" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="O189" s="14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="P189" s="12"/>
       <c r="Q189" s="12"/>
@@ -24479,78 +24497,86 @@
       <c r="AB189" s="12"/>
     </row>
     <row r="190">
-      <c r="A190" s="10" t="s">
-        <v>756</v>
-      </c>
-      <c r="B190" s="25" t="s">
-        <v>757</v>
-      </c>
-      <c r="C190" s="10" t="s">
-        <v>758</v>
-      </c>
-      <c r="D190" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="E190" s="9" t="s">
+      <c r="B190" s="23"/>
+      <c r="E190" s="43"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="C191" s="30" t="s">
+        <v>754</v>
+      </c>
+      <c r="D191" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="E191" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F190" s="12"/>
-      <c r="G190" s="12"/>
-      <c r="H190" s="12"/>
-      <c r="I190" s="12"/>
-      <c r="J190" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="K190" s="13">
-        <v>43620.0</v>
-      </c>
-      <c r="L190" s="12"/>
-      <c r="M190" s="10" t="s">
+      <c r="F191" s="59"/>
+      <c r="G191" s="59"/>
+      <c r="H191" s="59"/>
+      <c r="I191" s="59"/>
+      <c r="J191" s="59"/>
+      <c r="K191" s="42">
+        <v>45402.0</v>
+      </c>
+      <c r="L191" s="42"/>
+      <c r="M191" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="N190" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="O190" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="P190" s="12"/>
-      <c r="Q190" s="12"/>
-      <c r="R190" s="12"/>
-      <c r="S190" s="12"/>
-      <c r="T190" s="12"/>
-      <c r="U190" s="12"/>
-      <c r="V190" s="12"/>
-      <c r="W190" s="12"/>
-      <c r="X190" s="12"/>
-      <c r="Y190" s="12"/>
-      <c r="Z190" s="12"/>
-      <c r="AA190" s="12"/>
-      <c r="AB190" s="12"/>
-    </row>
-    <row r="191">
-      <c r="B191" s="23"/>
-      <c r="E191" s="43"/>
+      <c r="N191" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O191" s="59"/>
+      <c r="P191" s="59"/>
+      <c r="Q191" s="59"/>
+      <c r="R191" s="59"/>
+      <c r="S191" s="59"/>
+      <c r="T191" s="59"/>
+      <c r="U191" s="59"/>
+      <c r="V191" s="59"/>
+      <c r="W191" s="59"/>
+      <c r="X191" s="59"/>
+      <c r="Y191" s="59"/>
+      <c r="Z191" s="59"/>
+      <c r="AA191" s="59"/>
+      <c r="AB191" s="59"/>
     </row>
     <row r="192">
       <c r="A192" s="10" t="s">
-        <v>759</v>
-      </c>
-      <c r="B192" s="58"/>
-      <c r="C192" s="30"/>
-      <c r="D192" s="59"/>
-      <c r="E192" s="60"/>
+        <v>755</v>
+      </c>
+      <c r="B192" s="10" t="s">
+        <v>755</v>
+      </c>
+      <c r="C192" s="60" t="s">
+        <v>756</v>
+      </c>
+      <c r="D192" s="30" t="s">
+        <v>757</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F192" s="59"/>
       <c r="G192" s="59"/>
       <c r="H192" s="59"/>
       <c r="I192" s="59"/>
       <c r="J192" s="59"/>
-      <c r="K192" s="42"/>
+      <c r="K192" s="42">
+        <v>45402.0</v>
+      </c>
       <c r="L192" s="42"/>
       <c r="M192" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="N192" s="30"/>
+        <v>19</v>
+      </c>
+      <c r="N192" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="O192" s="59"/>
       <c r="P192" s="59"/>
       <c r="Q192" s="59"/>
@@ -24568,23 +24594,35 @@
     </row>
     <row r="193">
       <c r="A193" s="10" t="s">
-        <v>760</v>
-      </c>
-      <c r="B193" s="30"/>
-      <c r="C193" s="61"/>
-      <c r="D193" s="59"/>
-      <c r="E193" s="60"/>
+        <v>758</v>
+      </c>
+      <c r="B193" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="C193" s="60" t="s">
+        <v>759</v>
+      </c>
+      <c r="D193" s="30" t="s">
+        <v>757</v>
+      </c>
+      <c r="E193" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F193" s="59"/>
       <c r="G193" s="59"/>
       <c r="H193" s="59"/>
       <c r="I193" s="59"/>
       <c r="J193" s="59"/>
-      <c r="K193" s="42"/>
+      <c r="K193" s="42">
+        <v>45402.0</v>
+      </c>
       <c r="L193" s="42"/>
       <c r="M193" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="N193" s="30"/>
+        <v>19</v>
+      </c>
+      <c r="N193" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="O193" s="59"/>
       <c r="P193" s="59"/>
       <c r="Q193" s="59"/>
@@ -24602,57 +24640,81 @@
     </row>
     <row r="194">
       <c r="A194" s="10" t="s">
+        <v>760</v>
+      </c>
+      <c r="B194" s="10" t="s">
         <v>761</v>
       </c>
-      <c r="B194" s="61"/>
-      <c r="C194" s="30"/>
-      <c r="D194" s="59"/>
-      <c r="E194" s="60"/>
-      <c r="F194" s="59"/>
-      <c r="G194" s="59"/>
-      <c r="H194" s="59"/>
-      <c r="I194" s="59"/>
-      <c r="J194" s="59"/>
-      <c r="K194" s="42"/>
-      <c r="L194" s="42"/>
+      <c r="C194" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="D194" s="10" t="s">
+        <v>757</v>
+      </c>
+      <c r="E194" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F194" s="12"/>
+      <c r="G194" s="12"/>
+      <c r="H194" s="12"/>
+      <c r="I194" s="12"/>
+      <c r="J194" s="12"/>
+      <c r="K194" s="42">
+        <v>45402.0</v>
+      </c>
+      <c r="L194" s="12"/>
       <c r="M194" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="N194" s="30"/>
-      <c r="O194" s="59"/>
-      <c r="P194" s="59"/>
-      <c r="Q194" s="59"/>
-      <c r="R194" s="59"/>
-      <c r="S194" s="59"/>
-      <c r="T194" s="59"/>
-      <c r="U194" s="59"/>
-      <c r="V194" s="59"/>
-      <c r="W194" s="59"/>
-      <c r="X194" s="59"/>
-      <c r="Y194" s="59"/>
-      <c r="Z194" s="59"/>
-      <c r="AA194" s="59"/>
-      <c r="AB194" s="59"/>
+        <v>19</v>
+      </c>
+      <c r="N194" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O194" s="12"/>
+      <c r="P194" s="12"/>
+      <c r="Q194" s="12"/>
+      <c r="R194" s="12"/>
+      <c r="S194" s="12"/>
+      <c r="T194" s="12"/>
+      <c r="U194" s="12"/>
+      <c r="V194" s="12"/>
+      <c r="W194" s="12"/>
+      <c r="X194" s="12"/>
+      <c r="Y194" s="12"/>
+      <c r="Z194" s="12"/>
+      <c r="AA194" s="12"/>
+      <c r="AB194" s="12"/>
     </row>
     <row r="195">
       <c r="A195" s="10" t="s">
-        <v>762</v>
-      </c>
-      <c r="B195" s="23"/>
-      <c r="C195" s="12"/>
-      <c r="D195" s="12"/>
-      <c r="E195" s="43"/>
+        <v>763</v>
+      </c>
+      <c r="B195" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="C195" s="10" t="s">
+        <v>765</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="E195" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F195" s="12"/>
       <c r="G195" s="12"/>
       <c r="H195" s="12"/>
       <c r="I195" s="12"/>
       <c r="J195" s="12"/>
-      <c r="K195" s="12"/>
+      <c r="K195" s="42">
+        <v>45402.0</v>
+      </c>
       <c r="L195" s="12"/>
-      <c r="M195" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N195" s="12"/>
+      <c r="M195" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="N195" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="O195" s="12"/>
       <c r="P195" s="12"/>
       <c r="Q195" s="12"/>
@@ -24669,73 +24731,178 @@
       <c r="AB195" s="12"/>
     </row>
     <row r="196">
-      <c r="A196" s="10" t="s">
-        <v>763</v>
-      </c>
       <c r="B196" s="23"/>
-      <c r="C196" s="12"/>
-      <c r="D196" s="12"/>
       <c r="E196" s="43"/>
-      <c r="F196" s="12"/>
-      <c r="G196" s="12"/>
-      <c r="H196" s="12"/>
-      <c r="I196" s="12"/>
-      <c r="J196" s="12"/>
-      <c r="K196" s="12"/>
-      <c r="L196" s="12"/>
-      <c r="M196" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N196" s="12"/>
-      <c r="O196" s="12"/>
-      <c r="P196" s="12"/>
-      <c r="Q196" s="12"/>
-      <c r="R196" s="12"/>
-      <c r="S196" s="12"/>
-      <c r="T196" s="12"/>
-      <c r="U196" s="12"/>
-      <c r="V196" s="12"/>
-      <c r="W196" s="12"/>
-      <c r="X196" s="12"/>
-      <c r="Y196" s="12"/>
-      <c r="Z196" s="12"/>
-      <c r="AA196" s="12"/>
-      <c r="AB196" s="12"/>
     </row>
     <row r="197">
+      <c r="A197" s="9" t="s">
+        <v>767</v>
+      </c>
       <c r="B197" s="23"/>
       <c r="E197" s="43"/>
     </row>
     <row r="198">
       <c r="A198" s="10" t="s">
-        <v>764</v>
-      </c>
-      <c r="B198" s="23"/>
-      <c r="E198" s="43"/>
+        <v>768</v>
+      </c>
+      <c r="B198" s="25" t="s">
+        <v>768</v>
+      </c>
+      <c r="C198" s="10" t="s">
+        <v>769</v>
+      </c>
+      <c r="D198" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="E198" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F198" s="12"/>
+      <c r="G198" s="12"/>
+      <c r="H198" s="12"/>
+      <c r="I198" s="12"/>
+      <c r="J198" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K198" s="13">
+        <v>43620.0</v>
+      </c>
+      <c r="L198" s="12"/>
+      <c r="M198" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N198" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O198" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="P198" s="12"/>
+      <c r="Q198" s="12"/>
+      <c r="R198" s="12"/>
+      <c r="S198" s="12"/>
+      <c r="T198" s="12"/>
+      <c r="U198" s="12"/>
+      <c r="V198" s="12"/>
+      <c r="W198" s="12"/>
+      <c r="X198" s="12"/>
+      <c r="Y198" s="12"/>
+      <c r="Z198" s="12"/>
+      <c r="AA198" s="12"/>
+      <c r="AB198" s="12"/>
     </row>
     <row r="199">
-      <c r="B199" s="23"/>
-      <c r="E199" s="43"/>
+      <c r="A199" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="B199" s="25" t="s">
+        <v>772</v>
+      </c>
+      <c r="C199" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="D199" s="10" t="s">
+        <v>774</v>
+      </c>
+      <c r="E199" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F199" s="12"/>
+      <c r="G199" s="12"/>
+      <c r="H199" s="12"/>
+      <c r="I199" s="12"/>
+      <c r="J199" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K199" s="13">
+        <v>43620.0</v>
+      </c>
+      <c r="L199" s="12"/>
+      <c r="M199" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N199" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O199" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="P199" s="12"/>
+      <c r="Q199" s="12"/>
+      <c r="R199" s="12"/>
+      <c r="S199" s="12"/>
+      <c r="T199" s="12"/>
+      <c r="U199" s="12"/>
+      <c r="V199" s="12"/>
+      <c r="W199" s="12"/>
+      <c r="X199" s="12"/>
+      <c r="Y199" s="12"/>
+      <c r="Z199" s="12"/>
+      <c r="AA199" s="12"/>
+      <c r="AB199" s="12"/>
     </row>
     <row r="200">
-      <c r="A200" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="B200" s="23"/>
-      <c r="E200" s="43"/>
+      <c r="A200" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="B200" s="11" t="s">
+        <v>776</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="D200" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="E200" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F200" s="12"/>
+      <c r="G200" s="12"/>
+      <c r="H200" s="12"/>
+      <c r="I200" s="12"/>
+      <c r="J200" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K200" s="13">
+        <v>43620.0</v>
+      </c>
+      <c r="L200" s="12"/>
+      <c r="M200" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N200" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O200" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="P200" s="12"/>
+      <c r="Q200" s="12"/>
+      <c r="R200" s="12"/>
+      <c r="S200" s="12"/>
+      <c r="T200" s="12"/>
+      <c r="U200" s="12"/>
+      <c r="V200" s="12"/>
+      <c r="W200" s="12"/>
+      <c r="X200" s="12"/>
+      <c r="Y200" s="12"/>
+      <c r="Z200" s="12"/>
+      <c r="AA200" s="12"/>
+      <c r="AB200" s="12"/>
     </row>
     <row r="201">
       <c r="A201" s="10" t="s">
-        <v>766</v>
+        <v>779</v>
       </c>
       <c r="B201" s="25" t="s">
-        <v>766</v>
+        <v>780</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>767</v>
+        <v>781</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>768</v>
+        <v>782</v>
       </c>
       <c r="E201" s="9" t="s">
         <v>52</v>
@@ -24776,22 +24943,24 @@
     </row>
     <row r="202">
       <c r="A202" s="10" t="s">
-        <v>769</v>
+        <v>783</v>
       </c>
       <c r="B202" s="25" t="s">
-        <v>770</v>
+        <v>784</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>771</v>
+        <v>785</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>772</v>
+        <v>786</v>
       </c>
       <c r="E202" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F202" s="12"/>
-      <c r="G202" s="12"/>
+      <c r="G202" s="12" t="s">
+        <v>787</v>
+      </c>
       <c r="H202" s="12"/>
       <c r="I202" s="12"/>
       <c r="J202" s="29" t="s">
@@ -24826,16 +24995,16 @@
     </row>
     <row r="203">
       <c r="A203" s="10" t="s">
-        <v>773</v>
+        <v>788</v>
       </c>
       <c r="B203" s="11" t="s">
-        <v>774</v>
+        <v>789</v>
       </c>
       <c r="C203" s="10" t="s">
-        <v>775</v>
+        <v>790</v>
       </c>
       <c r="D203" s="10" t="s">
-        <v>776</v>
+        <v>786</v>
       </c>
       <c r="E203" s="9" t="s">
         <v>52</v>
@@ -24844,21 +25013,19 @@
       <c r="G203" s="12"/>
       <c r="H203" s="12"/>
       <c r="I203" s="12"/>
-      <c r="J203" s="29" t="s">
-        <v>162</v>
-      </c>
+      <c r="J203" s="19"/>
       <c r="K203" s="13">
-        <v>43620.0</v>
+        <v>44699.0</v>
       </c>
       <c r="L203" s="12"/>
       <c r="M203" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N203" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="O203" s="14" t="s">
-        <v>163</v>
+        <v>450</v>
       </c>
       <c r="P203" s="12"/>
       <c r="Q203" s="12"/>
@@ -24876,16 +25043,16 @@
     </row>
     <row r="204">
       <c r="A204" s="10" t="s">
-        <v>777</v>
+        <v>791</v>
       </c>
       <c r="B204" s="25" t="s">
-        <v>778</v>
+        <v>791</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>779</v>
+        <v>792</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="E204" s="9" t="s">
         <v>52</v>
@@ -24926,24 +25093,22 @@
     </row>
     <row r="205">
       <c r="A205" s="10" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
       <c r="B205" s="25" t="s">
-        <v>782</v>
+        <v>793</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>783</v>
+        <v>794</v>
       </c>
       <c r="D205" s="10" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="E205" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F205" s="12"/>
-      <c r="G205" s="12" t="s">
-        <v>785</v>
-      </c>
+      <c r="G205" s="12"/>
       <c r="H205" s="12"/>
       <c r="I205" s="12"/>
       <c r="J205" s="29" t="s">
@@ -24978,16 +25143,16 @@
     </row>
     <row r="206">
       <c r="A206" s="10" t="s">
-        <v>786</v>
-      </c>
-      <c r="B206" s="11" t="s">
-        <v>787</v>
+        <v>795</v>
+      </c>
+      <c r="B206" s="25" t="s">
+        <v>796</v>
       </c>
       <c r="C206" s="10" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="D206" s="10" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E206" s="9" t="s">
         <v>52</v>
@@ -24996,19 +25161,21 @@
       <c r="G206" s="12"/>
       <c r="H206" s="12"/>
       <c r="I206" s="12"/>
-      <c r="J206" s="19"/>
+      <c r="J206" s="29" t="s">
+        <v>162</v>
+      </c>
       <c r="K206" s="13">
-        <v>44699.0</v>
+        <v>43620.0</v>
       </c>
       <c r="L206" s="12"/>
       <c r="M206" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N206" s="10" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="O206" s="14" t="s">
-        <v>450</v>
+        <v>163</v>
       </c>
       <c r="P206" s="12"/>
       <c r="Q206" s="12"/>
@@ -25026,16 +25193,16 @@
     </row>
     <row r="207">
       <c r="A207" s="10" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="B207" s="25" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="D207" s="10" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="E207" s="9" t="s">
         <v>52</v>
@@ -25076,16 +25243,16 @@
     </row>
     <row r="208">
       <c r="A208" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="B208" s="25" t="s">
-        <v>791</v>
+        <v>800</v>
+      </c>
+      <c r="B208" s="11" t="s">
+        <v>801</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>792</v>
+        <v>802</v>
       </c>
       <c r="D208" s="10" t="s">
-        <v>784</v>
+        <v>803</v>
       </c>
       <c r="E208" s="9" t="s">
         <v>52</v>
@@ -25094,21 +25261,19 @@
       <c r="G208" s="12"/>
       <c r="H208" s="12"/>
       <c r="I208" s="12"/>
-      <c r="J208" s="29" t="s">
-        <v>162</v>
-      </c>
+      <c r="J208" s="19"/>
       <c r="K208" s="13">
-        <v>43620.0</v>
+        <v>44699.0</v>
       </c>
       <c r="L208" s="12"/>
       <c r="M208" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N208" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="O208" s="14" t="s">
-        <v>163</v>
+        <v>450</v>
       </c>
       <c r="P208" s="12"/>
       <c r="Q208" s="12"/>
@@ -25125,67 +25290,29 @@
       <c r="AB208" s="12"/>
     </row>
     <row r="209">
-      <c r="A209" s="10" t="s">
-        <v>793</v>
-      </c>
-      <c r="B209" s="25" t="s">
-        <v>794</v>
-      </c>
-      <c r="C209" s="10" t="s">
-        <v>795</v>
-      </c>
-      <c r="D209" s="10" t="s">
-        <v>780</v>
-      </c>
-      <c r="E209" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F209" s="12"/>
-      <c r="G209" s="12"/>
-      <c r="H209" s="12"/>
-      <c r="I209" s="12"/>
-      <c r="J209" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="K209" s="13">
-        <v>43620.0</v>
-      </c>
-      <c r="L209" s="12"/>
-      <c r="M209" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N209" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="O209" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="P209" s="12"/>
-      <c r="Q209" s="12"/>
-      <c r="R209" s="12"/>
-      <c r="S209" s="12"/>
-      <c r="T209" s="12"/>
-      <c r="U209" s="12"/>
-      <c r="V209" s="12"/>
-      <c r="W209" s="12"/>
-      <c r="X209" s="12"/>
-      <c r="Y209" s="12"/>
-      <c r="Z209" s="12"/>
-      <c r="AA209" s="12"/>
-      <c r="AB209" s="12"/>
+      <c r="A209" s="10"/>
+      <c r="B209" s="25"/>
+      <c r="C209" s="10"/>
+      <c r="D209" s="10"/>
+      <c r="E209" s="9"/>
+      <c r="J209" s="19"/>
+      <c r="K209" s="13"/>
+      <c r="M209" s="10"/>
+      <c r="N209" s="10"/>
+      <c r="O209" s="10"/>
     </row>
     <row r="210">
       <c r="A210" s="10" t="s">
-        <v>796</v>
+        <v>804</v>
       </c>
       <c r="B210" s="25" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="C210" s="10" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="D210" s="10" t="s">
-        <v>776</v>
+        <v>807</v>
       </c>
       <c r="E210" s="9" t="s">
         <v>52</v>
@@ -25200,12 +25327,14 @@
       <c r="K210" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L210" s="12"/>
+      <c r="L210" s="13">
+        <v>45402.0</v>
+      </c>
       <c r="M210" s="10" t="s">
-        <v>19</v>
+        <v>808</v>
       </c>
       <c r="N210" s="10" t="s">
-        <v>96</v>
+        <v>809</v>
       </c>
       <c r="O210" s="14" t="s">
         <v>163</v>
@@ -25226,38 +25355,34 @@
     </row>
     <row r="211">
       <c r="A211" s="10" t="s">
-        <v>798</v>
-      </c>
-      <c r="B211" s="11" t="s">
-        <v>799</v>
+        <v>276</v>
+      </c>
+      <c r="B211" s="10" t="s">
+        <v>276</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>800</v>
+        <v>810</v>
       </c>
       <c r="D211" s="10" t="s">
-        <v>801</v>
-      </c>
-      <c r="E211" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="E211" s="10" t="s">
         <v>52</v>
       </c>
       <c r="F211" s="12"/>
       <c r="G211" s="12"/>
       <c r="H211" s="12"/>
       <c r="I211" s="12"/>
-      <c r="J211" s="19"/>
-      <c r="K211" s="13">
-        <v>44699.0</v>
-      </c>
+      <c r="J211" s="12"/>
+      <c r="K211" s="12"/>
       <c r="L211" s="12"/>
       <c r="M211" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N211" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O211" s="14" t="s">
-        <v>450</v>
-      </c>
+        <v>812</v>
+      </c>
+      <c r="O211" s="12"/>
       <c r="P211" s="12"/>
       <c r="Q211" s="12"/>
       <c r="R211" s="12"/>
@@ -25273,25 +25398,320 @@
       <c r="AB211" s="12"/>
     </row>
     <row r="212">
-      <c r="B212" s="23"/>
+      <c r="A212" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="C212" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="D212" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E212" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F212" s="12"/>
+      <c r="G212" s="12"/>
+      <c r="H212" s="12"/>
+      <c r="I212" s="12"/>
+      <c r="J212" s="12"/>
+      <c r="K212" s="12"/>
+      <c r="L212" s="12"/>
+      <c r="M212" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N212" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="O212" s="12"/>
+      <c r="P212" s="12"/>
+      <c r="Q212" s="12"/>
+      <c r="R212" s="12"/>
+      <c r="S212" s="12"/>
+      <c r="T212" s="12"/>
+      <c r="U212" s="12"/>
+      <c r="V212" s="12"/>
+      <c r="W212" s="12"/>
+      <c r="X212" s="12"/>
+      <c r="Y212" s="12"/>
+      <c r="Z212" s="12"/>
+      <c r="AA212" s="12"/>
+      <c r="AB212" s="12"/>
     </row>
     <row r="213">
-      <c r="B213" s="23"/>
+      <c r="A213" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="B213" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="C213" s="10" t="s">
+        <v>816</v>
+      </c>
+      <c r="D213" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E213" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F213" s="12"/>
+      <c r="G213" s="12"/>
+      <c r="H213" s="12"/>
+      <c r="I213" s="12"/>
+      <c r="J213" s="12"/>
+      <c r="K213" s="12"/>
+      <c r="L213" s="12"/>
+      <c r="M213" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N213" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="O213" s="12"/>
+      <c r="P213" s="12"/>
+      <c r="Q213" s="12"/>
+      <c r="R213" s="12"/>
+      <c r="S213" s="12"/>
+      <c r="T213" s="12"/>
+      <c r="U213" s="12"/>
+      <c r="V213" s="12"/>
+      <c r="W213" s="12"/>
+      <c r="X213" s="12"/>
+      <c r="Y213" s="12"/>
+      <c r="Z213" s="12"/>
+      <c r="AA213" s="12"/>
+      <c r="AB213" s="12"/>
     </row>
     <row r="214">
-      <c r="B214" s="23"/>
+      <c r="A214" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="B214" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="C214" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="D214" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E214" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F214" s="12"/>
+      <c r="G214" s="12"/>
+      <c r="H214" s="12"/>
+      <c r="I214" s="12"/>
+      <c r="J214" s="12"/>
+      <c r="K214" s="12"/>
+      <c r="L214" s="12"/>
+      <c r="M214" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N214" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="O214" s="12"/>
+      <c r="P214" s="12"/>
+      <c r="Q214" s="12"/>
+      <c r="R214" s="12"/>
+      <c r="S214" s="12"/>
+      <c r="T214" s="12"/>
+      <c r="U214" s="12"/>
+      <c r="V214" s="12"/>
+      <c r="W214" s="12"/>
+      <c r="X214" s="12"/>
+      <c r="Y214" s="12"/>
+      <c r="Z214" s="12"/>
+      <c r="AA214" s="12"/>
+      <c r="AB214" s="12"/>
     </row>
     <row r="215">
-      <c r="B215" s="23"/>
+      <c r="A215" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="B215" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="C215" s="10" t="s">
+        <v>821</v>
+      </c>
+      <c r="D215" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E215" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F215" s="12"/>
+      <c r="G215" s="12"/>
+      <c r="H215" s="12"/>
+      <c r="I215" s="12"/>
+      <c r="J215" s="12"/>
+      <c r="K215" s="12"/>
+      <c r="L215" s="12"/>
+      <c r="M215" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N215" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="O215" s="12"/>
+      <c r="P215" s="12"/>
+      <c r="Q215" s="12"/>
+      <c r="R215" s="12"/>
+      <c r="S215" s="12"/>
+      <c r="T215" s="12"/>
+      <c r="U215" s="12"/>
+      <c r="V215" s="12"/>
+      <c r="W215" s="12"/>
+      <c r="X215" s="12"/>
+      <c r="Y215" s="12"/>
+      <c r="Z215" s="12"/>
+      <c r="AA215" s="12"/>
+      <c r="AB215" s="12"/>
     </row>
     <row r="216">
-      <c r="B216" s="23"/>
+      <c r="A216" s="10" t="s">
+        <v>822</v>
+      </c>
+      <c r="B216" s="10" t="s">
+        <v>822</v>
+      </c>
+      <c r="C216" s="10" t="s">
+        <v>823</v>
+      </c>
+      <c r="D216" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E216" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F216" s="12"/>
+      <c r="G216" s="12"/>
+      <c r="H216" s="12"/>
+      <c r="I216" s="12"/>
+      <c r="J216" s="12"/>
+      <c r="K216" s="12"/>
+      <c r="L216" s="12"/>
+      <c r="M216" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N216" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="O216" s="12"/>
+      <c r="P216" s="12"/>
+      <c r="Q216" s="12"/>
+      <c r="R216" s="12"/>
+      <c r="S216" s="12"/>
+      <c r="T216" s="12"/>
+      <c r="U216" s="12"/>
+      <c r="V216" s="12"/>
+      <c r="W216" s="12"/>
+      <c r="X216" s="12"/>
+      <c r="Y216" s="12"/>
+      <c r="Z216" s="12"/>
+      <c r="AA216" s="12"/>
+      <c r="AB216" s="12"/>
     </row>
     <row r="217">
-      <c r="B217" s="23"/>
+      <c r="A217" s="10" t="s">
+        <v>824</v>
+      </c>
+      <c r="B217" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="C217" s="10" t="s">
+        <v>826</v>
+      </c>
+      <c r="D217" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E217" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F217" s="12"/>
+      <c r="G217" s="12"/>
+      <c r="H217" s="12"/>
+      <c r="I217" s="12"/>
+      <c r="J217" s="12"/>
+      <c r="K217" s="12"/>
+      <c r="L217" s="12"/>
+      <c r="M217" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N217" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="O217" s="12"/>
+      <c r="P217" s="12"/>
+      <c r="Q217" s="12"/>
+      <c r="R217" s="12"/>
+      <c r="S217" s="12"/>
+      <c r="T217" s="12"/>
+      <c r="U217" s="12"/>
+      <c r="V217" s="12"/>
+      <c r="W217" s="12"/>
+      <c r="X217" s="12"/>
+      <c r="Y217" s="12"/>
+      <c r="Z217" s="12"/>
+      <c r="AA217" s="12"/>
+      <c r="AB217" s="12"/>
     </row>
     <row r="218">
-      <c r="B218" s="23"/>
+      <c r="A218" s="10" t="s">
+        <v>827</v>
+      </c>
+      <c r="B218" s="25" t="s">
+        <v>828</v>
+      </c>
+      <c r="C218" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="D218" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E218" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F218" s="12"/>
+      <c r="G218" s="12"/>
+      <c r="H218" s="12"/>
+      <c r="I218" s="12"/>
+      <c r="J218" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="K218" s="13">
+        <v>43620.0</v>
+      </c>
+      <c r="L218" s="13">
+        <v>45402.0</v>
+      </c>
+      <c r="M218" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="N218" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="O218" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="P218" s="12"/>
+      <c r="Q218" s="12"/>
+      <c r="R218" s="12"/>
+      <c r="S218" s="12"/>
+      <c r="T218" s="12"/>
+      <c r="U218" s="12"/>
+      <c r="V218" s="12"/>
+      <c r="W218" s="12"/>
+      <c r="X218" s="12"/>
+      <c r="Y218" s="12"/>
+      <c r="Z218" s="12"/>
+      <c r="AA218" s="12"/>
+      <c r="AB218" s="12"/>
     </row>
     <row r="219">
       <c r="B219" s="23"/>
@@ -27765,26 +28185,20 @@
     <row r="1042">
       <c r="B1042" s="23"/>
     </row>
-    <row r="1043">
-      <c r="B1043" s="23"/>
-    </row>
-    <row r="1044">
-      <c r="B1044" s="23"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AB994">
+  <conditionalFormatting sqref="A2:AB992">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB994">
+  <conditionalFormatting sqref="A2:AB992">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB994">
+  <conditionalFormatting sqref="A2:AB992">
     <cfRule type="expression" dxfId="4" priority="3">
-      <formula>$M2="changed"</formula>
+      <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -28022,131 +28436,131 @@
     <hyperlink r:id="rId232" ref="O129"/>
     <hyperlink r:id="rId233" ref="J130"/>
     <hyperlink r:id="rId234" ref="O130"/>
-    <hyperlink r:id="rId235" ref="J131"/>
-    <hyperlink r:id="rId236" ref="O131"/>
-    <hyperlink r:id="rId237" ref="J132"/>
-    <hyperlink r:id="rId238" ref="O132"/>
-    <hyperlink r:id="rId239" ref="J133"/>
-    <hyperlink r:id="rId240" ref="O133"/>
-    <hyperlink r:id="rId241" ref="J134"/>
-    <hyperlink r:id="rId242" ref="O134"/>
-    <hyperlink r:id="rId243" ref="J135"/>
-    <hyperlink r:id="rId244" ref="O135"/>
-    <hyperlink r:id="rId245" ref="J136"/>
-    <hyperlink r:id="rId246" ref="O136"/>
-    <hyperlink r:id="rId247" ref="J137"/>
-    <hyperlink r:id="rId248" ref="O137"/>
-    <hyperlink r:id="rId249" ref="J138"/>
-    <hyperlink r:id="rId250" ref="O138"/>
-    <hyperlink r:id="rId251" ref="J139"/>
-    <hyperlink r:id="rId252" ref="O139"/>
-    <hyperlink r:id="rId253" ref="J140"/>
-    <hyperlink r:id="rId254" ref="O140"/>
-    <hyperlink r:id="rId255" ref="J141"/>
-    <hyperlink r:id="rId256" ref="O141"/>
-    <hyperlink r:id="rId257" ref="J142"/>
-    <hyperlink r:id="rId258" ref="O142"/>
-    <hyperlink r:id="rId259" ref="J143"/>
-    <hyperlink r:id="rId260" ref="O143"/>
-    <hyperlink r:id="rId261" ref="J144"/>
-    <hyperlink r:id="rId262" ref="O144"/>
-    <hyperlink r:id="rId263" ref="J145"/>
-    <hyperlink r:id="rId264" ref="O145"/>
-    <hyperlink r:id="rId265" ref="J148"/>
-    <hyperlink r:id="rId266" ref="O148"/>
-    <hyperlink r:id="rId267" ref="O149"/>
-    <hyperlink r:id="rId268" ref="J150"/>
-    <hyperlink r:id="rId269" ref="O150"/>
-    <hyperlink r:id="rId270" ref="J151"/>
-    <hyperlink r:id="rId271" ref="O151"/>
-    <hyperlink r:id="rId272" ref="J152"/>
-    <hyperlink r:id="rId273" ref="O152"/>
-    <hyperlink r:id="rId274" ref="J153"/>
-    <hyperlink r:id="rId275" ref="O153"/>
-    <hyperlink r:id="rId276" ref="O154"/>
-    <hyperlink r:id="rId277" ref="J155"/>
-    <hyperlink r:id="rId278" ref="O155"/>
-    <hyperlink r:id="rId279" ref="J156"/>
-    <hyperlink r:id="rId280" ref="O156"/>
-    <hyperlink r:id="rId281" ref="J157"/>
-    <hyperlink r:id="rId282" ref="O157"/>
-    <hyperlink r:id="rId283" ref="J158"/>
-    <hyperlink r:id="rId284" ref="O158"/>
-    <hyperlink r:id="rId285" ref="J159"/>
-    <hyperlink r:id="rId286" ref="O159"/>
-    <hyperlink r:id="rId287" ref="J160"/>
-    <hyperlink r:id="rId288" ref="O160"/>
-    <hyperlink r:id="rId289" ref="J161"/>
-    <hyperlink r:id="rId290" ref="O161"/>
-    <hyperlink r:id="rId291" ref="J162"/>
-    <hyperlink r:id="rId292" ref="O162"/>
-    <hyperlink r:id="rId293" ref="J163"/>
-    <hyperlink r:id="rId294" ref="O163"/>
-    <hyperlink r:id="rId295" ref="J164"/>
-    <hyperlink r:id="rId296" ref="O164"/>
-    <hyperlink r:id="rId297" ref="J165"/>
-    <hyperlink r:id="rId298" ref="O165"/>
-    <hyperlink r:id="rId299" ref="J166"/>
-    <hyperlink r:id="rId300" ref="O166"/>
-    <hyperlink r:id="rId301" ref="O167"/>
-    <hyperlink r:id="rId302" ref="J168"/>
-    <hyperlink r:id="rId303" ref="O168"/>
-    <hyperlink r:id="rId304" ref="J169"/>
-    <hyperlink r:id="rId305" ref="O169"/>
-    <hyperlink r:id="rId306" ref="J170"/>
-    <hyperlink r:id="rId307" ref="O170"/>
-    <hyperlink r:id="rId308" ref="J171"/>
-    <hyperlink r:id="rId309" ref="O171"/>
-    <hyperlink r:id="rId310" ref="J172"/>
-    <hyperlink r:id="rId311" ref="O172"/>
-    <hyperlink r:id="rId312" ref="J173"/>
-    <hyperlink r:id="rId313" ref="O173"/>
-    <hyperlink r:id="rId314" ref="J174"/>
-    <hyperlink r:id="rId315" ref="O174"/>
-    <hyperlink r:id="rId316" ref="J175"/>
-    <hyperlink r:id="rId317" ref="O175"/>
-    <hyperlink r:id="rId318" ref="O176"/>
-    <hyperlink r:id="rId319" ref="J177"/>
-    <hyperlink r:id="rId320" ref="O177"/>
-    <hyperlink r:id="rId321" ref="J178"/>
-    <hyperlink r:id="rId322" ref="O178"/>
-    <hyperlink r:id="rId323" ref="O179"/>
-    <hyperlink r:id="rId324" ref="J180"/>
-    <hyperlink r:id="rId325" ref="O180"/>
-    <hyperlink r:id="rId326" ref="O181"/>
-    <hyperlink r:id="rId327" ref="O182"/>
-    <hyperlink r:id="rId328" ref="O183"/>
-    <hyperlink r:id="rId329" ref="O184"/>
-    <hyperlink r:id="rId330" ref="O185"/>
-    <hyperlink r:id="rId331" ref="J186"/>
-    <hyperlink r:id="rId332" ref="O186"/>
-    <hyperlink r:id="rId333" ref="J187"/>
-    <hyperlink r:id="rId334" ref="O187"/>
-    <hyperlink r:id="rId335" ref="J188"/>
-    <hyperlink r:id="rId336" ref="O188"/>
-    <hyperlink r:id="rId337" ref="O189"/>
-    <hyperlink r:id="rId338" ref="J190"/>
-    <hyperlink r:id="rId339" ref="O190"/>
-    <hyperlink r:id="rId340" ref="J201"/>
-    <hyperlink r:id="rId341" ref="O201"/>
-    <hyperlink r:id="rId342" ref="J202"/>
-    <hyperlink r:id="rId343" ref="O202"/>
-    <hyperlink r:id="rId344" ref="J203"/>
-    <hyperlink r:id="rId345" ref="O203"/>
-    <hyperlink r:id="rId346" ref="J204"/>
-    <hyperlink r:id="rId347" ref="O204"/>
-    <hyperlink r:id="rId348" ref="J205"/>
-    <hyperlink r:id="rId349" ref="O205"/>
-    <hyperlink r:id="rId350" ref="O206"/>
-    <hyperlink r:id="rId351" ref="J207"/>
-    <hyperlink r:id="rId352" ref="O207"/>
-    <hyperlink r:id="rId353" ref="J208"/>
-    <hyperlink r:id="rId354" ref="O208"/>
-    <hyperlink r:id="rId355" ref="J209"/>
-    <hyperlink r:id="rId356" ref="O209"/>
-    <hyperlink r:id="rId357" ref="J210"/>
-    <hyperlink r:id="rId358" ref="O210"/>
-    <hyperlink r:id="rId359" ref="O211"/>
+    <hyperlink r:id="rId235" ref="J132"/>
+    <hyperlink r:id="rId236" ref="O132"/>
+    <hyperlink r:id="rId237" ref="J133"/>
+    <hyperlink r:id="rId238" ref="O133"/>
+    <hyperlink r:id="rId239" ref="J134"/>
+    <hyperlink r:id="rId240" ref="O134"/>
+    <hyperlink r:id="rId241" ref="J135"/>
+    <hyperlink r:id="rId242" ref="O135"/>
+    <hyperlink r:id="rId243" ref="J136"/>
+    <hyperlink r:id="rId244" ref="O136"/>
+    <hyperlink r:id="rId245" ref="J137"/>
+    <hyperlink r:id="rId246" ref="O137"/>
+    <hyperlink r:id="rId247" ref="J138"/>
+    <hyperlink r:id="rId248" ref="O138"/>
+    <hyperlink r:id="rId249" ref="J139"/>
+    <hyperlink r:id="rId250" ref="O139"/>
+    <hyperlink r:id="rId251" ref="J140"/>
+    <hyperlink r:id="rId252" ref="O140"/>
+    <hyperlink r:id="rId253" ref="J141"/>
+    <hyperlink r:id="rId254" ref="O141"/>
+    <hyperlink r:id="rId255" ref="J142"/>
+    <hyperlink r:id="rId256" ref="O142"/>
+    <hyperlink r:id="rId257" ref="J143"/>
+    <hyperlink r:id="rId258" ref="O143"/>
+    <hyperlink r:id="rId259" ref="J144"/>
+    <hyperlink r:id="rId260" ref="O144"/>
+    <hyperlink r:id="rId261" ref="J145"/>
+    <hyperlink r:id="rId262" ref="O145"/>
+    <hyperlink r:id="rId263" ref="J148"/>
+    <hyperlink r:id="rId264" ref="O148"/>
+    <hyperlink r:id="rId265" ref="O149"/>
+    <hyperlink r:id="rId266" ref="J150"/>
+    <hyperlink r:id="rId267" ref="O150"/>
+    <hyperlink r:id="rId268" ref="J151"/>
+    <hyperlink r:id="rId269" ref="O151"/>
+    <hyperlink r:id="rId270" ref="J152"/>
+    <hyperlink r:id="rId271" ref="O152"/>
+    <hyperlink r:id="rId272" ref="J153"/>
+    <hyperlink r:id="rId273" ref="O153"/>
+    <hyperlink r:id="rId274" ref="O154"/>
+    <hyperlink r:id="rId275" ref="J155"/>
+    <hyperlink r:id="rId276" ref="O155"/>
+    <hyperlink r:id="rId277" ref="J156"/>
+    <hyperlink r:id="rId278" ref="O156"/>
+    <hyperlink r:id="rId279" ref="J157"/>
+    <hyperlink r:id="rId280" ref="O157"/>
+    <hyperlink r:id="rId281" ref="J158"/>
+    <hyperlink r:id="rId282" ref="O158"/>
+    <hyperlink r:id="rId283" ref="J159"/>
+    <hyperlink r:id="rId284" ref="O159"/>
+    <hyperlink r:id="rId285" ref="J160"/>
+    <hyperlink r:id="rId286" ref="O160"/>
+    <hyperlink r:id="rId287" ref="J161"/>
+    <hyperlink r:id="rId288" ref="O161"/>
+    <hyperlink r:id="rId289" ref="J162"/>
+    <hyperlink r:id="rId290" ref="O162"/>
+    <hyperlink r:id="rId291" ref="J163"/>
+    <hyperlink r:id="rId292" ref="O163"/>
+    <hyperlink r:id="rId293" ref="J164"/>
+    <hyperlink r:id="rId294" ref="O164"/>
+    <hyperlink r:id="rId295" ref="J165"/>
+    <hyperlink r:id="rId296" ref="O165"/>
+    <hyperlink r:id="rId297" ref="O166"/>
+    <hyperlink r:id="rId298" ref="J167"/>
+    <hyperlink r:id="rId299" ref="O167"/>
+    <hyperlink r:id="rId300" ref="J168"/>
+    <hyperlink r:id="rId301" ref="O168"/>
+    <hyperlink r:id="rId302" ref="J169"/>
+    <hyperlink r:id="rId303" ref="O169"/>
+    <hyperlink r:id="rId304" ref="J170"/>
+    <hyperlink r:id="rId305" ref="O170"/>
+    <hyperlink r:id="rId306" ref="J171"/>
+    <hyperlink r:id="rId307" ref="O171"/>
+    <hyperlink r:id="rId308" ref="J172"/>
+    <hyperlink r:id="rId309" ref="O172"/>
+    <hyperlink r:id="rId310" ref="J173"/>
+    <hyperlink r:id="rId311" ref="O173"/>
+    <hyperlink r:id="rId312" ref="J174"/>
+    <hyperlink r:id="rId313" ref="O174"/>
+    <hyperlink r:id="rId314" ref="O175"/>
+    <hyperlink r:id="rId315" ref="J176"/>
+    <hyperlink r:id="rId316" ref="O176"/>
+    <hyperlink r:id="rId317" ref="J177"/>
+    <hyperlink r:id="rId318" ref="O177"/>
+    <hyperlink r:id="rId319" ref="O178"/>
+    <hyperlink r:id="rId320" ref="J179"/>
+    <hyperlink r:id="rId321" ref="O179"/>
+    <hyperlink r:id="rId322" ref="O180"/>
+    <hyperlink r:id="rId323" ref="O181"/>
+    <hyperlink r:id="rId324" ref="O182"/>
+    <hyperlink r:id="rId325" ref="O183"/>
+    <hyperlink r:id="rId326" ref="O184"/>
+    <hyperlink r:id="rId327" ref="J185"/>
+    <hyperlink r:id="rId328" ref="O185"/>
+    <hyperlink r:id="rId329" ref="J186"/>
+    <hyperlink r:id="rId330" ref="O186"/>
+    <hyperlink r:id="rId331" ref="J187"/>
+    <hyperlink r:id="rId332" ref="O187"/>
+    <hyperlink r:id="rId333" ref="O188"/>
+    <hyperlink r:id="rId334" ref="J189"/>
+    <hyperlink r:id="rId335" ref="O189"/>
+    <hyperlink r:id="rId336" ref="J198"/>
+    <hyperlink r:id="rId337" ref="O198"/>
+    <hyperlink r:id="rId338" ref="J199"/>
+    <hyperlink r:id="rId339" ref="O199"/>
+    <hyperlink r:id="rId340" ref="J200"/>
+    <hyperlink r:id="rId341" ref="O200"/>
+    <hyperlink r:id="rId342" ref="J201"/>
+    <hyperlink r:id="rId343" ref="O201"/>
+    <hyperlink r:id="rId344" ref="J202"/>
+    <hyperlink r:id="rId345" ref="O202"/>
+    <hyperlink r:id="rId346" ref="O203"/>
+    <hyperlink r:id="rId347" ref="J204"/>
+    <hyperlink r:id="rId348" ref="O204"/>
+    <hyperlink r:id="rId349" ref="J205"/>
+    <hyperlink r:id="rId350" ref="O205"/>
+    <hyperlink r:id="rId351" ref="J206"/>
+    <hyperlink r:id="rId352" ref="O206"/>
+    <hyperlink r:id="rId353" ref="J207"/>
+    <hyperlink r:id="rId354" ref="O207"/>
+    <hyperlink r:id="rId355" ref="O208"/>
+    <hyperlink r:id="rId356" ref="J210"/>
+    <hyperlink r:id="rId357" ref="O210"/>
+    <hyperlink r:id="rId358" ref="J218"/>
+    <hyperlink r:id="rId359" ref="O218"/>
   </hyperlinks>
   <drawing r:id="rId360"/>
 </worksheet>
@@ -28197,110 +28611,110 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J3" s="19"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J5" s="19"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J8" s="19"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>802</v>
+        <v>830</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="13"/>

</xml_diff>

<commit_message>
adds AI Act documentation; fixes pd concept
- adds EU AI Act documentation with message on vocabulary being in early
  stages (diagrams are missing)
- fixes 'Country' being defined twice in PD (removes the later addition
  from @besteves4)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/pd.xlsx
+++ b/code/vocab_csv/pd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="840">
   <si>
     <t>Term</t>
   </si>
@@ -25477,48 +25477,46 @@
       <c r="AB210" s="12"/>
     </row>
     <row r="211">
-      <c r="A211" s="10" t="s">
+      <c r="A211" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="B211" s="10" t="s">
+      <c r="B211" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="C211" s="10" t="s">
+      <c r="C211" s="35" t="s">
         <v>819</v>
       </c>
-      <c r="D211" s="10" t="s">
+      <c r="D211" s="35" t="s">
         <v>820</v>
       </c>
-      <c r="E211" s="10" t="s">
+      <c r="E211" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F211" s="12"/>
-      <c r="G211" s="12"/>
-      <c r="H211" s="12"/>
-      <c r="I211" s="12"/>
-      <c r="J211" s="12"/>
-      <c r="K211" s="12"/>
-      <c r="L211" s="12"/>
-      <c r="M211" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N211" s="10" t="s">
+      <c r="F211" s="37"/>
+      <c r="G211" s="37"/>
+      <c r="H211" s="37"/>
+      <c r="I211" s="37"/>
+      <c r="J211" s="37"/>
+      <c r="K211" s="37"/>
+      <c r="L211" s="37"/>
+      <c r="M211" s="35"/>
+      <c r="N211" s="35" t="s">
         <v>821</v>
       </c>
-      <c r="O211" s="12"/>
-      <c r="P211" s="12"/>
-      <c r="Q211" s="12"/>
-      <c r="R211" s="12"/>
-      <c r="S211" s="12"/>
-      <c r="T211" s="12"/>
-      <c r="U211" s="12"/>
-      <c r="V211" s="12"/>
-      <c r="W211" s="12"/>
-      <c r="X211" s="12"/>
-      <c r="Y211" s="12"/>
-      <c r="Z211" s="12"/>
-      <c r="AA211" s="12"/>
-      <c r="AB211" s="12"/>
+      <c r="O211" s="37"/>
+      <c r="P211" s="37"/>
+      <c r="Q211" s="37"/>
+      <c r="R211" s="37"/>
+      <c r="S211" s="37"/>
+      <c r="T211" s="37"/>
+      <c r="U211" s="37"/>
+      <c r="V211" s="37"/>
+      <c r="W211" s="37"/>
+      <c r="X211" s="37"/>
+      <c r="Y211" s="37"/>
+      <c r="Z211" s="37"/>
+      <c r="AA211" s="37"/>
+      <c r="AB211" s="37"/>
     </row>
     <row r="212">
       <c r="A212" s="10" t="s">

</xml_diff>

<commit_message>
Adds Location concepts to PD #341
- adds location concepts to PD for HomeLocation, WorkLocation, and
  CurrentLocation (needs to be reviewed and confirmed)
- changes parent for existing location concepts so that all locations are
  instances of `dpv:Location` in addition to being personal data
- includes RDF and HTML with note on usage

Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/pd.xlsx
+++ b/code/vocab_csv/pd.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="929">
   <si>
     <t>Term</t>
   </si>
@@ -910,6 +910,9 @@
     <t>pd:Location</t>
   </si>
   <si>
+    <t>dpv:PersonalData,dpv:Location</t>
+  </si>
+  <si>
     <t>BirthCountry</t>
   </si>
   <si>
@@ -919,10 +922,7 @@
     <t>Information about country of birth</t>
   </si>
   <si>
-    <t>pd:BirthPlace</t>
-  </si>
-  <si>
-    <t>use pd:BirthCountry</t>
+    <t>pd:BirthPlace,pd:Country</t>
   </si>
   <si>
     <t>Harshvardhan J. Pandit, Beatriz Esteves</t>
@@ -1678,6 +1678,9 @@
     <t>Information about location expressed using Global Position System coordinates (GPS)</t>
   </si>
   <si>
+    <t>pd:CurrentLocation</t>
+  </si>
+  <si>
     <t>GroupMembership</t>
   </si>
   <si>
@@ -2730,6 +2733,9 @@
     <t>dpv:Country</t>
   </si>
   <si>
+    <t>use pd:BirthCountry</t>
+  </si>
+  <si>
     <t>Special Categories</t>
   </si>
   <si>
@@ -2914,6 +2920,33 @@
   </si>
   <si>
     <t>Information about location expressed as room number or similar numbering systems</t>
+  </si>
+  <si>
+    <t>HomeLocation</t>
+  </si>
+  <si>
+    <t>Home Place</t>
+  </si>
+  <si>
+    <t>Information about a person's home place, including their location, address, and locality</t>
+  </si>
+  <si>
+    <t>WorkLocation</t>
+  </si>
+  <si>
+    <t>Work Place</t>
+  </si>
+  <si>
+    <t>Information about a person's work place, including their location, address, and locality</t>
+  </si>
+  <si>
+    <t>CurrentLocation</t>
+  </si>
+  <si>
+    <t>Current Location</t>
+  </si>
+  <si>
+    <t>Information about a person's current location (e.g. by asking the address, using GPS)</t>
   </si>
   <si>
     <t>dpv:SpecialCategoryPersonalData</t>
@@ -15835,10 +15868,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="29.88"/>
-    <col customWidth="1" min="3" max="3" width="54.25"/>
+    <col customWidth="1" min="1" max="1" width="29.88"/>
+    <col customWidth="1" min="2" max="2" width="13.0"/>
+    <col customWidth="1" min="3" max="3" width="6.75"/>
     <col customWidth="1" min="4" max="4" width="22.25"/>
-    <col customWidth="1" min="10" max="10" width="67.5"/>
+    <col customWidth="1" min="10" max="10" width="3.38"/>
     <col customWidth="1" min="14" max="14" width="62.25"/>
   </cols>
   <sheetData>
@@ -15902,7 +15936,7 @@
       <c r="D2" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F2" s="12"/>
@@ -15952,7 +15986,7 @@
       <c r="D3" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F3" s="12"/>
@@ -16002,7 +16036,7 @@
       <c r="D4" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="12"/>
@@ -16054,7 +16088,7 @@
       <c r="D5" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="12"/>
@@ -16104,7 +16138,7 @@
       <c r="D6" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="12"/>
@@ -16152,7 +16186,7 @@
       <c r="D7" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F7" s="12"/>
@@ -16200,7 +16234,7 @@
       <c r="D8" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="12"/>
@@ -16250,7 +16284,7 @@
       <c r="D9" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="12"/>
@@ -16300,7 +16334,7 @@
       <c r="D10" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F10" s="12"/>
@@ -16352,7 +16386,7 @@
       <c r="D11" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="12"/>
@@ -16402,7 +16436,7 @@
       <c r="D12" s="49" t="s">
         <v>259</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="50"/>
@@ -16454,7 +16488,7 @@
       <c r="D13" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="12"/>
@@ -16504,7 +16538,7 @@
       <c r="D14" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="12"/>
@@ -16558,7 +16592,7 @@
       <c r="D15" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="12"/>
@@ -16606,8 +16640,8 @@
       <c r="D16" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>50</v>
+      <c r="E16" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -16617,9 +16651,11 @@
       <c r="K16" s="13">
         <v>44671.0</v>
       </c>
-      <c r="L16" s="12"/>
+      <c r="L16" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M16" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N16" s="10" t="s">
         <v>20</v>
@@ -16643,33 +16679,33 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>283</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="10" t="s">
-        <v>287</v>
-      </c>
+      <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="43">
         <v>45504.0</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="30" t="s">
-        <v>19</v>
+      <c r="L17" s="13">
+        <v>46063.0</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="N17" s="10" t="s">
         <v>288</v>
@@ -16702,7 +16738,7 @@
       <c r="D18" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="12"/>
@@ -16752,7 +16788,7 @@
       <c r="D19" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="12"/>
@@ -16802,7 +16838,7 @@
       <c r="D20" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="12"/>
@@ -16852,7 +16888,7 @@
       <c r="D21" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F21" s="12"/>
@@ -16906,7 +16942,7 @@
       <c r="D22" s="52" t="s">
         <v>300</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F22" s="50"/>
@@ -16958,7 +16994,7 @@
       <c r="D23" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F23" s="12"/>
@@ -17010,7 +17046,7 @@
       <c r="D24" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F24" s="12"/>
@@ -17060,7 +17096,7 @@
       <c r="D25" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="12"/>
@@ -17110,7 +17146,7 @@
       <c r="D26" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F26" s="12"/>
@@ -17160,7 +17196,7 @@
       <c r="D27" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="12"/>
@@ -17212,7 +17248,7 @@
       <c r="D28" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="12"/>
@@ -17262,7 +17298,7 @@
       <c r="D29" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="10"/>
@@ -17314,8 +17350,8 @@
       <c r="D30" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>50</v>
+      <c r="E30" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -17327,9 +17363,11 @@
       <c r="K30" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L30" s="12"/>
+      <c r="L30" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M30" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N30" s="10" t="s">
         <v>111</v>
@@ -17364,7 +17402,7 @@
       <c r="D31" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="12"/>
@@ -17414,7 +17452,7 @@
       <c r="D32" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="12"/>
@@ -17464,7 +17502,7 @@
       <c r="D33" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="12"/>
@@ -17514,7 +17552,7 @@
       <c r="D34" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="12"/>
@@ -17564,7 +17602,7 @@
       <c r="D35" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F35" s="12"/>
@@ -17614,7 +17652,7 @@
       <c r="D36" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F36" s="12"/>
@@ -17664,7 +17702,7 @@
       <c r="D37" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="12"/>
@@ -17714,7 +17752,7 @@
       <c r="D38" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F38" s="12"/>
@@ -17766,7 +17804,7 @@
       <c r="D39" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F39" s="12"/>
@@ -17816,7 +17854,7 @@
       <c r="D40" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F40" s="12"/>
@@ -17866,7 +17904,7 @@
       <c r="D41" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F41" s="12"/>
@@ -17914,7 +17952,7 @@
       <c r="D42" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F42" s="12"/>
@@ -17964,7 +18002,7 @@
       <c r="D43" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F43" s="12"/>
@@ -18012,7 +18050,7 @@
       <c r="D44" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F44" s="12"/>
@@ -18064,7 +18102,7 @@
       <c r="D45" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F45" s="12"/>
@@ -18114,7 +18152,7 @@
       <c r="D46" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F46" s="50"/>
@@ -18164,7 +18202,7 @@
       <c r="D47" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="10"/>
@@ -18216,7 +18254,7 @@
       <c r="D48" s="52" t="s">
         <v>387</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F48" s="50"/>
@@ -18266,7 +18304,7 @@
       <c r="D49" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F49" s="50"/>
@@ -18316,7 +18354,7 @@
       <c r="D50" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F50" s="12"/>
@@ -18366,7 +18404,7 @@
       <c r="D51" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F51" s="12"/>
@@ -18414,7 +18452,7 @@
       <c r="D52" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F52" s="12"/>
@@ -18464,7 +18502,7 @@
       <c r="D53" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="12"/>
@@ -18514,7 +18552,7 @@
       <c r="D54" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E54" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F54" s="12"/>
@@ -18564,7 +18602,7 @@
       <c r="D55" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F55" s="12"/>
@@ -18614,7 +18652,7 @@
       <c r="D56" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F56" s="12"/>
@@ -18664,7 +18702,7 @@
       <c r="D57" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F57" s="12"/>
@@ -18714,7 +18752,7 @@
       <c r="D58" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F58" s="12"/>
@@ -18762,7 +18800,7 @@
       <c r="D59" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F59" s="12"/>
@@ -18810,7 +18848,7 @@
       <c r="D60" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F60" s="12"/>
@@ -18858,7 +18896,7 @@
       <c r="D61" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F61" s="12"/>
@@ -18904,7 +18942,7 @@
       <c r="D62" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F62" s="12"/>
@@ -18954,7 +18992,7 @@
       <c r="D63" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E63" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F63" s="12"/>
@@ -19002,7 +19040,7 @@
       <c r="D64" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F64" s="12"/>
@@ -19050,7 +19088,7 @@
       <c r="D65" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F65" s="12"/>
@@ -19100,7 +19138,7 @@
       <c r="D66" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F66" s="12"/>
@@ -19146,7 +19184,7 @@
       <c r="D67" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E67" s="9" t="s">
+      <c r="E67" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F67" s="12"/>
@@ -19196,7 +19234,7 @@
       <c r="D68" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="E68" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F68" s="12"/>
@@ -19246,7 +19284,7 @@
       <c r="D69" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="E69" s="9" t="s">
+      <c r="E69" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F69" s="12"/>
@@ -19294,7 +19332,7 @@
       <c r="D70" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F70" s="12"/>
@@ -19340,7 +19378,7 @@
       <c r="D71" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E71" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F71" s="12"/>
@@ -19390,7 +19428,7 @@
       <c r="D72" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E72" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F72" s="12"/>
@@ -19440,7 +19478,7 @@
       <c r="D73" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F73" s="12"/>
@@ -19490,7 +19528,7 @@
       <c r="D74" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F74" s="12"/>
@@ -19542,7 +19580,7 @@
       <c r="D75" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E75" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F75" s="12"/>
@@ -19594,7 +19632,7 @@
       <c r="D76" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F76" s="12"/>
@@ -19646,7 +19684,7 @@
       <c r="D77" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F77" s="12"/>
@@ -19698,7 +19736,7 @@
       <c r="D78" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E78" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F78" s="12"/>
@@ -19748,7 +19786,7 @@
       <c r="D79" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="E79" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F79" s="12"/>
@@ -19798,7 +19836,7 @@
       <c r="D80" s="10" t="s">
         <v>500</v>
       </c>
-      <c r="E80" s="9" t="s">
+      <c r="E80" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F80" s="12"/>
@@ -19848,7 +19886,7 @@
       <c r="D81" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="E81" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F81" s="12"/>
@@ -19896,7 +19934,7 @@
       <c r="D82" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E82" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F82" s="12"/>
@@ -19946,7 +19984,7 @@
       <c r="D83" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E83" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F83" s="12"/>
@@ -19996,7 +20034,7 @@
       <c r="D84" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="E84" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F84" s="12"/>
@@ -20046,7 +20084,7 @@
       <c r="D85" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E85" s="9" t="s">
+      <c r="E85" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F85" s="12"/>
@@ -20096,7 +20134,7 @@
       <c r="D86" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="E86" s="9" t="s">
+      <c r="E86" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F86" s="12"/>
@@ -20144,7 +20182,7 @@
       <c r="D87" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E87" s="9" t="s">
+      <c r="E87" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F87" s="12"/>
@@ -20192,10 +20230,10 @@
         <v>522</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>50</v>
+        <v>523</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
@@ -20207,9 +20245,11 @@
       <c r="K88" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L88" s="12"/>
+      <c r="L88" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M88" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N88" s="10" t="s">
         <v>111</v>
@@ -20233,18 +20273,18 @@
     </row>
     <row r="89">
       <c r="A89" s="10" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D89" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="E89" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F89" s="12"/>
@@ -20283,18 +20323,18 @@
     </row>
     <row r="90">
       <c r="A90" s="10" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C90" s="47" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D90" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E90" s="9" t="s">
+      <c r="E90" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F90" s="12"/>
@@ -20335,23 +20375,23 @@
     </row>
     <row r="91">
       <c r="A91" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D91" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E91" s="9" t="s">
+      <c r="E91" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F91" s="12"/>
       <c r="G91" s="12" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
@@ -20387,18 +20427,18 @@
     </row>
     <row r="92">
       <c r="A92" s="10" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E92" s="9" t="s">
+      <c r="E92" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F92" s="12"/>
@@ -20437,18 +20477,18 @@
     </row>
     <row r="93">
       <c r="A93" s="10" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D93" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E93" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F93" s="12"/>
@@ -20487,18 +20527,18 @@
     </row>
     <row r="94">
       <c r="A94" s="10" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C94" s="47" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E94" s="9" t="s">
+      <c r="E94" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F94" s="12"/>
@@ -20537,18 +20577,18 @@
     </row>
     <row r="95">
       <c r="A95" s="10" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="E95" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F95" s="12"/>
@@ -20587,18 +20627,18 @@
     </row>
     <row r="96">
       <c r="A96" s="10" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="E96" s="9" t="s">
+      <c r="E96" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F96" s="12"/>
@@ -20635,18 +20675,18 @@
     </row>
     <row r="97">
       <c r="A97" s="10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D97" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E97" s="9" t="s">
+      <c r="E97" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F97" s="12"/>
@@ -20683,18 +20723,18 @@
     </row>
     <row r="98">
       <c r="A98" s="10" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D98" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E98" s="9" t="s">
+      <c r="E98" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F98" s="12"/>
@@ -20733,18 +20773,18 @@
     </row>
     <row r="99">
       <c r="A99" s="10" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E99" s="9" t="s">
+      <c r="E99" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F99" s="12"/>
@@ -20783,18 +20823,18 @@
     </row>
     <row r="100">
       <c r="A100" s="10" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E100" s="9" t="s">
+      <c r="E100" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F100" s="12"/>
@@ -20833,18 +20873,18 @@
     </row>
     <row r="101">
       <c r="A101" s="10" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="E101" s="9" t="s">
+      <c r="E101" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F101" s="12"/>
@@ -20883,18 +20923,18 @@
     </row>
     <row r="102">
       <c r="A102" s="10" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D102" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="E102" s="9" t="s">
+      <c r="E102" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F102" s="12"/>
@@ -20931,18 +20971,18 @@
     </row>
     <row r="103">
       <c r="A103" s="10" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="E103" s="9" t="s">
+      <c r="E103" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F103" s="12"/>
@@ -20981,18 +21021,18 @@
     </row>
     <row r="104">
       <c r="A104" s="10" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D104" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E104" s="9" t="s">
+      <c r="E104" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F104" s="12"/>
@@ -21031,18 +21071,18 @@
     </row>
     <row r="105">
       <c r="A105" s="10" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D105" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="E105" s="9" t="s">
+      <c r="E105" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F105" s="12"/>
@@ -21081,18 +21121,18 @@
     </row>
     <row r="106">
       <c r="A106" s="10" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="E106" s="9" t="s">
+      <c r="E106" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F106" s="12"/>
@@ -21131,18 +21171,18 @@
     </row>
     <row r="107">
       <c r="A107" s="10" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E107" s="9" t="s">
+      <c r="E107" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F107" s="12"/>
@@ -21181,18 +21221,18 @@
     </row>
     <row r="108">
       <c r="A108" s="10" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D108" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E108" s="9" t="s">
+      <c r="E108" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F108" s="12"/>
@@ -21231,18 +21271,18 @@
     </row>
     <row r="109">
       <c r="A109" s="10" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D109" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E109" s="9" t="s">
+      <c r="E109" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F109" s="12"/>
@@ -21283,18 +21323,18 @@
     </row>
     <row r="110">
       <c r="A110" s="10" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>579</v>
-      </c>
-      <c r="E110" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="E110" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F110" s="12"/>
@@ -21333,18 +21373,18 @@
     </row>
     <row r="111">
       <c r="A111" s="10" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D111" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="E111" s="9" t="s">
+      <c r="E111" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F111" s="12"/>
@@ -21383,23 +21423,23 @@
     </row>
     <row r="112">
       <c r="A112" s="10" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E112" s="9" t="s">
+      <c r="E112" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F112" s="12"/>
       <c r="G112" s="12" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
@@ -21437,18 +21477,18 @@
     </row>
     <row r="113">
       <c r="A113" s="10" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E113" s="9" t="s">
+      <c r="E113" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F113" s="12"/>
@@ -21487,23 +21527,23 @@
     </row>
     <row r="114">
       <c r="A114" s="10" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D114" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E114" s="9" t="s">
-        <v>50</v>
+      <c r="E114" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F114" s="12"/>
       <c r="G114" s="12" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
@@ -21513,9 +21553,11 @@
       <c r="K114" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L114" s="12"/>
+      <c r="L114" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M114" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N114" s="10" t="s">
         <v>111</v>
@@ -21539,18 +21581,18 @@
     </row>
     <row r="115">
       <c r="A115" s="10" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D115" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="E115" s="9" t="s">
+      <c r="E115" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F115" s="12"/>
@@ -21589,18 +21631,18 @@
     </row>
     <row r="116">
       <c r="A116" s="10" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D116" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E116" s="9" t="s">
+      <c r="E116" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F116" s="12"/>
@@ -21639,18 +21681,18 @@
     </row>
     <row r="117">
       <c r="A117" s="10" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D117" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="E117" s="9" t="s">
+      <c r="E117" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F117" s="12"/>
@@ -21689,18 +21731,18 @@
     </row>
     <row r="118">
       <c r="A118" s="10" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D118" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="E118" s="9" t="s">
+      <c r="E118" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F118" s="12"/>
@@ -21739,18 +21781,18 @@
     </row>
     <row r="119">
       <c r="A119" s="10" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D119" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E119" s="9" t="s">
+      <c r="E119" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F119" s="12"/>
@@ -21785,18 +21827,18 @@
     </row>
     <row r="120">
       <c r="A120" s="10" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="E120" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E120" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F120" s="12"/>
@@ -21835,18 +21877,18 @@
     </row>
     <row r="121">
       <c r="A121" s="10" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D121" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E121" s="9" t="s">
+      <c r="E121" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F121" s="12"/>
@@ -21881,23 +21923,23 @@
     </row>
     <row r="122">
       <c r="A122" s="10" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="E122" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E122" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F122" s="12"/>
       <c r="G122" s="12" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="H122" s="12"/>
       <c r="I122" s="12"/>
@@ -21933,18 +21975,18 @@
     </row>
     <row r="123">
       <c r="A123" s="10" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D123" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="E123" s="9" t="s">
+      <c r="E123" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F123" s="12"/>
@@ -21983,18 +22025,18 @@
     </row>
     <row r="124">
       <c r="A124" s="10" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D124" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="E124" s="9" t="s">
+      <c r="E124" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F124" s="12"/>
@@ -22033,18 +22075,18 @@
     </row>
     <row r="125">
       <c r="A125" s="10" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D125" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="E125" s="9" t="s">
+      <c r="E125" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F125" s="12"/>
@@ -22083,18 +22125,18 @@
     </row>
     <row r="126">
       <c r="A126" s="10" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D126" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="E126" s="9" t="s">
+      <c r="E126" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F126" s="12"/>
@@ -22133,18 +22175,18 @@
     </row>
     <row r="127">
       <c r="A127" s="10" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D127" s="10" t="s">
-        <v>624</v>
-      </c>
-      <c r="E127" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="E127" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F127" s="12"/>
@@ -22181,18 +22223,18 @@
     </row>
     <row r="128">
       <c r="A128" s="10" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>627</v>
-      </c>
-      <c r="E128" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="E128" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F128" s="12"/>
@@ -22231,18 +22273,18 @@
     </row>
     <row r="129">
       <c r="A129" s="54" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B129" s="55" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C129" s="54" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D129" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="E129" s="9" t="s">
+      <c r="E129" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F129" s="50"/>
@@ -22250,7 +22292,7 @@
       <c r="H129" s="50"/>
       <c r="I129" s="50"/>
       <c r="J129" s="26" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="K129" s="51">
         <v>44139.0</v>
@@ -22281,18 +22323,18 @@
     </row>
     <row r="130">
       <c r="A130" s="54" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B130" s="55" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C130" s="52" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D130" s="52" t="s">
-        <v>635</v>
-      </c>
-      <c r="E130" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="E130" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F130" s="50"/>
@@ -22300,7 +22342,7 @@
       <c r="H130" s="50"/>
       <c r="I130" s="50"/>
       <c r="J130" s="26" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="K130" s="51">
         <v>44139.0</v>
@@ -22331,18 +22373,18 @@
     </row>
     <row r="131">
       <c r="A131" s="54" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B131" s="55" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C131" s="54" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D131" s="52" t="s">
-        <v>640</v>
-      </c>
-      <c r="E131" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="E131" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F131" s="50"/>
@@ -22350,7 +22392,7 @@
       <c r="H131" s="50"/>
       <c r="I131" s="50"/>
       <c r="J131" s="26" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="K131" s="51">
         <v>44139.0</v>
@@ -22381,18 +22423,18 @@
     </row>
     <row r="132">
       <c r="A132" s="10" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D132" s="10" t="s">
-        <v>645</v>
-      </c>
-      <c r="E132" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="E132" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F132" s="12"/>
@@ -22431,18 +22473,18 @@
     </row>
     <row r="133">
       <c r="A133" s="10" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D133" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E133" s="9" t="s">
+      <c r="E133" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F133" s="12"/>
@@ -22479,18 +22521,18 @@
     </row>
     <row r="134">
       <c r="A134" s="10" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E134" s="9" t="s">
+      <c r="E134" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F134" s="12"/>
@@ -22531,18 +22573,18 @@
     </row>
     <row r="135">
       <c r="A135" s="10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="E135" s="9" t="s">
+      <c r="E135" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F135" s="12"/>
@@ -22581,23 +22623,23 @@
     </row>
     <row r="137">
       <c r="A137" s="10" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D137" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E137" s="9" t="s">
+      <c r="E137" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F137" s="12"/>
       <c r="G137" s="12" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="H137" s="12"/>
       <c r="I137" s="12"/>
@@ -22633,18 +22675,18 @@
     </row>
     <row r="138">
       <c r="A138" s="10" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D138" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="E138" s="9" t="s">
+      <c r="E138" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F138" s="12"/>
@@ -22683,18 +22725,18 @@
     </row>
     <row r="139">
       <c r="A139" s="10" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B139" s="25" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D139" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E139" s="9" t="s">
+      <c r="E139" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F139" s="12"/>
@@ -22733,18 +22775,18 @@
     </row>
     <row r="140">
       <c r="A140" s="10" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B140" s="25" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D140" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="E140" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E140" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F140" s="12"/>
@@ -22783,18 +22825,18 @@
     </row>
     <row r="141">
       <c r="A141" s="10" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C141" s="47" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D141" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E141" s="9" t="s">
+      <c r="E141" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F141" s="12"/>
@@ -22833,18 +22875,18 @@
     </row>
     <row r="142">
       <c r="A142" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>627</v>
-      </c>
-      <c r="E142" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="E142" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F142" s="12"/>
@@ -22883,23 +22925,23 @@
     </row>
     <row r="143">
       <c r="A143" s="10" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B143" s="25" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D143" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E143" s="9" t="s">
+      <c r="E143" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F143" s="12"/>
       <c r="G143" s="12" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="H143" s="12"/>
       <c r="I143" s="12"/>
@@ -22935,18 +22977,18 @@
     </row>
     <row r="144">
       <c r="A144" s="10" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B144" s="25" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D144" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E144" s="9" t="s">
+      <c r="E144" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F144" s="12"/>
@@ -22985,18 +23027,18 @@
     </row>
     <row r="145">
       <c r="A145" s="10" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="D145" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="E145" s="9" t="s">
+      <c r="E145" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F145" s="12"/>
@@ -23035,18 +23077,18 @@
     </row>
     <row r="146">
       <c r="A146" s="10" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D146" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="E146" s="9" t="s">
+      <c r="E146" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F146" s="12"/>
@@ -23087,18 +23129,18 @@
     </row>
     <row r="147">
       <c r="A147" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B147" s="25" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D147" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E147" s="9" t="s">
+      <c r="E147" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F147" s="12"/>
@@ -23137,18 +23179,18 @@
     </row>
     <row r="148">
       <c r="A148" s="10" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D148" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E148" s="9" t="s">
+      <c r="E148" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F148" s="12"/>
@@ -23187,18 +23229,18 @@
     </row>
     <row r="149">
       <c r="A149" s="10" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D149" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E149" s="9" t="s">
+      <c r="E149" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F149" s="12"/>
@@ -23237,19 +23279,19 @@
     </row>
     <row r="150">
       <c r="A150" s="10" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D150" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E150" s="9" t="s">
-        <v>692</v>
+      <c r="E150" s="10" t="s">
+        <v>693</v>
       </c>
       <c r="F150" s="12"/>
       <c r="G150" s="12"/>
@@ -23264,7 +23306,7 @@
         <v>19</v>
       </c>
       <c r="N150" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="O150" s="10"/>
       <c r="P150" s="12"/>
@@ -23283,18 +23325,18 @@
     </row>
     <row r="151">
       <c r="A151" s="10" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B151" s="25" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D151" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E151" s="9" t="s">
+      <c r="E151" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F151" s="12"/>
@@ -23333,18 +23375,18 @@
     </row>
     <row r="152">
       <c r="A152" s="10" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D152" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E152" s="9" t="s">
+      <c r="E152" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F152" s="12"/>
@@ -23379,18 +23421,18 @@
     </row>
     <row r="153">
       <c r="A153" s="10" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D153" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="E153" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="E153" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F153" s="12"/>
@@ -23425,18 +23467,18 @@
     </row>
     <row r="154">
       <c r="A154" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>706</v>
+      </c>
+      <c r="C154" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="D154" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="B154" s="11" t="s">
-        <v>705</v>
-      </c>
-      <c r="C154" s="10" t="s">
-        <v>706</v>
-      </c>
-      <c r="D154" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="E154" s="9" t="s">
+      <c r="E154" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F154" s="12"/>
@@ -23471,18 +23513,18 @@
     </row>
     <row r="155">
       <c r="A155" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B155" s="25" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D155" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E155" s="9" t="s">
+      <c r="E155" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F155" s="12"/>
@@ -23521,18 +23563,18 @@
     </row>
     <row r="156">
       <c r="A156" s="10" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B156" s="11" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D156" s="10" t="s">
-        <v>713</v>
-      </c>
-      <c r="E156" s="9" t="s">
+        <v>714</v>
+      </c>
+      <c r="E156" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F156" s="12"/>
@@ -23569,23 +23611,23 @@
     </row>
     <row r="157">
       <c r="A157" s="10" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D157" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E157" s="9" t="s">
+      <c r="E157" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F157" s="10"/>
       <c r="G157" s="10" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="H157" s="12"/>
       <c r="I157" s="12"/>
@@ -23621,18 +23663,18 @@
     </row>
     <row r="158">
       <c r="A158" s="10" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D158" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E158" s="9" t="s">
+      <c r="E158" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F158" s="12"/>
@@ -23671,18 +23713,18 @@
     </row>
     <row r="159">
       <c r="A159" s="10" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B159" s="25" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D159" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E159" s="9" t="s">
+      <c r="E159" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F159" s="12"/>
@@ -23721,18 +23763,18 @@
     </row>
     <row r="160">
       <c r="A160" s="10" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B160" s="25" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D160" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="E160" s="9" t="s">
+      <c r="E160" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F160" s="12"/>
@@ -23771,18 +23813,18 @@
     </row>
     <row r="161">
       <c r="A161" s="10" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D161" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E161" s="9" t="s">
+      <c r="E161" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F161" s="12"/>
@@ -23821,18 +23863,18 @@
     </row>
     <row r="162">
       <c r="A162" s="10" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B162" s="25" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="D162" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="E162" s="9" t="s">
+      <c r="E162" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F162" s="12"/>
@@ -23871,18 +23913,18 @@
     </row>
     <row r="163">
       <c r="A163" s="10" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D163" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E163" s="9" t="s">
+      <c r="E163" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F163" s="12"/>
@@ -23921,18 +23963,18 @@
     </row>
     <row r="164">
       <c r="A164" s="10" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B164" s="25" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D164" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E164" s="9" t="s">
+      <c r="E164" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F164" s="12"/>
@@ -23971,18 +24013,18 @@
     </row>
     <row r="165">
       <c r="A165" s="10" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D165" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E165" s="9" t="s">
+      <c r="E165" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F165" s="12"/>
@@ -24021,18 +24063,18 @@
     </row>
     <row r="166">
       <c r="A166" s="10" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B166" s="25" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D166" s="10" t="s">
-        <v>627</v>
-      </c>
-      <c r="E166" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="E166" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F166" s="12"/>
@@ -24071,18 +24113,18 @@
     </row>
     <row r="167">
       <c r="A167" s="10" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E167" s="9" t="s">
+      <c r="E167" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F167" s="12"/>
@@ -24090,7 +24132,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="12"/>
       <c r="J167" s="16" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="K167" s="13">
         <v>43795.0</v>
@@ -24102,10 +24144,10 @@
         <v>157</v>
       </c>
       <c r="N167" s="10" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="O167" s="14" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="P167" s="12"/>
       <c r="Q167" s="12"/>
@@ -24123,18 +24165,18 @@
     </row>
     <row r="168">
       <c r="A168" s="10" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B168" s="25" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D168" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="E168" s="9" t="s">
+      <c r="E168" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F168" s="12"/>
@@ -24173,18 +24215,18 @@
     </row>
     <row r="169">
       <c r="A169" s="10" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D169" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="E169" s="9" t="s">
+      <c r="E169" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F169" s="12"/>
@@ -24223,18 +24265,18 @@
     </row>
     <row r="170">
       <c r="A170" s="10" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C170" s="48" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D170" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="E170" s="9" t="s">
+      <c r="E170" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F170" s="12"/>
@@ -24273,18 +24315,18 @@
     </row>
     <row r="171">
       <c r="A171" s="10" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D171" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E171" s="9" t="s">
+      <c r="E171" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F171" s="12"/>
@@ -24323,23 +24365,23 @@
     </row>
     <row r="172">
       <c r="A172" s="10" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B172" s="25" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C172" s="48" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D172" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="E172" s="9" t="s">
+      <c r="E172" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F172" s="12"/>
       <c r="G172" s="12" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="H172" s="12"/>
       <c r="I172" s="12"/>
@@ -24375,18 +24417,18 @@
     </row>
     <row r="173">
       <c r="A173" s="10" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>761</v>
-      </c>
-      <c r="E173" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="E173" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F173" s="12"/>
@@ -24402,7 +24444,7 @@
         <v>19</v>
       </c>
       <c r="N173" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="O173" s="30"/>
       <c r="P173" s="12"/>
@@ -24421,18 +24463,18 @@
     </row>
     <row r="174">
       <c r="A174" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D174" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="E174" s="9" t="s">
+      <c r="E174" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F174" s="12"/>
@@ -24469,18 +24511,18 @@
     </row>
     <row r="175">
       <c r="A175" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B175" s="25" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D175" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E175" s="9" t="s">
+      <c r="E175" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F175" s="12"/>
@@ -24519,18 +24561,18 @@
     </row>
     <row r="176">
       <c r="A176" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D176" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E176" s="9" t="s">
+      <c r="E176" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F176" s="12"/>
@@ -24569,18 +24611,18 @@
     </row>
     <row r="177">
       <c r="A177" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="D177" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E177" s="9" t="s">
+      <c r="E177" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F177" s="12"/>
@@ -24619,18 +24661,18 @@
     </row>
     <row r="178">
       <c r="A178" s="10" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B178" s="25" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D178" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E178" s="9" t="s">
+      <c r="E178" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F178" s="12"/>
@@ -24669,18 +24711,18 @@
     </row>
     <row r="179">
       <c r="A179" s="10" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>778</v>
-      </c>
-      <c r="E179" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="E179" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F179" s="12"/>
@@ -24696,7 +24738,7 @@
         <v>19</v>
       </c>
       <c r="N179" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="O179" s="10"/>
       <c r="P179" s="12"/>
@@ -24715,18 +24757,18 @@
     </row>
     <row r="180">
       <c r="A180" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B180" s="25" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C180" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D180" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="E180" s="9" t="s">
+      <c r="E180" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F180" s="12"/>
@@ -24765,18 +24807,18 @@
     </row>
     <row r="181">
       <c r="A181" s="48" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B181" s="59" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C181" s="47" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>778</v>
-      </c>
-      <c r="E181" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="E181" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F181" s="12"/>
@@ -24815,18 +24857,18 @@
     </row>
     <row r="182">
       <c r="A182" s="10" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B182" s="23" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D182" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E182" s="9" t="s">
+      <c r="E182" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F182" s="12"/>
@@ -24865,18 +24907,18 @@
     </row>
     <row r="183">
       <c r="A183" s="10" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D183" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="E183" s="9" t="s">
+      <c r="E183" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F183" s="12"/>
@@ -24915,19 +24957,19 @@
     </row>
     <row r="184">
       <c r="A184" s="10" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D184" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="E184" s="9" t="s">
-        <v>50</v>
+      <c r="E184" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F184" s="12"/>
       <c r="G184" s="12"/>
@@ -24937,9 +24979,11 @@
       <c r="K184" s="13">
         <v>44671.0</v>
       </c>
-      <c r="L184" s="12"/>
+      <c r="L184" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M184" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N184" s="10" t="s">
         <v>20</v>
@@ -24963,18 +25007,18 @@
     </row>
     <row r="185">
       <c r="A185" s="10" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>794</v>
-      </c>
-      <c r="E185" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="E185" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F185" s="12"/>
@@ -24982,7 +25026,7 @@
       <c r="H185" s="12"/>
       <c r="I185" s="12"/>
       <c r="J185" s="16" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="K185" s="13">
         <v>43795.0</v>
@@ -24994,10 +25038,10 @@
         <v>157</v>
       </c>
       <c r="N185" s="10" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="O185" s="14" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="P185" s="12"/>
       <c r="Q185" s="12"/>
@@ -25015,23 +25059,23 @@
     </row>
     <row r="186">
       <c r="A186" s="10" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B186" s="25" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="E186" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E186" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F186" s="10"/>
       <c r="G186" s="10" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="H186" s="12"/>
       <c r="I186" s="12"/>
@@ -25067,18 +25111,18 @@
     </row>
     <row r="187">
       <c r="A187" s="10" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B187" s="30" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C187" s="60" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="D187" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="E187" s="9" t="s">
+      <c r="E187" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F187" s="61"/>
@@ -25115,18 +25159,18 @@
     </row>
     <row r="188">
       <c r="A188" s="10" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B188" s="25" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="E188" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E188" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F188" s="12"/>
@@ -25165,18 +25209,18 @@
     </row>
     <row r="189">
       <c r="A189" s="10" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B189" s="11" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>807</v>
-      </c>
-      <c r="E189" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="E189" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F189" s="12"/>
@@ -25213,18 +25257,18 @@
     </row>
     <row r="190">
       <c r="A190" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="B190" s="11" t="s">
+        <v>810</v>
+      </c>
+      <c r="C190" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="D190" s="10" t="s">
         <v>808</v>
       </c>
-      <c r="B190" s="11" t="s">
-        <v>809</v>
-      </c>
-      <c r="C190" s="10" t="s">
-        <v>810</v>
-      </c>
-      <c r="D190" s="10" t="s">
-        <v>807</v>
-      </c>
-      <c r="E190" s="9" t="s">
+      <c r="E190" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F190" s="12"/>
@@ -25261,18 +25305,18 @@
     </row>
     <row r="191">
       <c r="A191" s="10" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B191" s="11" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="D191" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="E191" s="9" t="s">
+      <c r="E191" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F191" s="12"/>
@@ -25309,18 +25353,18 @@
     </row>
     <row r="192">
       <c r="A192" s="10" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B192" s="11" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C192" s="10" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D192" s="10" t="s">
-        <v>816</v>
-      </c>
-      <c r="E192" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="E192" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F192" s="12"/>
@@ -25357,18 +25401,18 @@
     </row>
     <row r="193">
       <c r="A193" s="10" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B193" s="11" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>820</v>
-      </c>
-      <c r="E193" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="E193" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F193" s="12"/>
@@ -25407,18 +25451,18 @@
     </row>
     <row r="194">
       <c r="A194" s="10" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B194" s="25" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C194" s="48" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="D194" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="E194" s="9" t="s">
+      <c r="E194" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F194" s="12"/>
@@ -25457,18 +25501,18 @@
     </row>
     <row r="195">
       <c r="A195" s="10" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B195" s="25" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="D195" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="E195" s="9" t="s">
+      <c r="E195" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F195" s="12"/>
@@ -25507,18 +25551,18 @@
     </row>
     <row r="196">
       <c r="A196" s="10" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B196" s="25" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D196" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E196" s="9" t="s">
+      <c r="E196" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F196" s="12"/>
@@ -25557,18 +25601,18 @@
     </row>
     <row r="197">
       <c r="A197" s="10" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B197" s="11" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C197" s="10" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D197" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E197" s="9" t="s">
+      <c r="E197" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F197" s="12"/>
@@ -25605,18 +25649,18 @@
     </row>
     <row r="198">
       <c r="A198" s="10" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B198" s="11" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C198" s="10" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>835</v>
-      </c>
-      <c r="E198" s="9" t="s">
+        <v>836</v>
+      </c>
+      <c r="E198" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F198" s="12"/>
@@ -25632,7 +25676,7 @@
         <v>19</v>
       </c>
       <c r="N198" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="O198" s="10"/>
       <c r="P198" s="12"/>
@@ -25651,18 +25695,18 @@
     </row>
     <row r="199">
       <c r="A199" s="10" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B199" s="25" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D199" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E199" s="9" t="s">
+      <c r="E199" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F199" s="12"/>
@@ -25701,22 +25745,21 @@
     </row>
     <row r="200">
       <c r="B200" s="23"/>
-      <c r="E200" s="44"/>
     </row>
     <row r="201">
       <c r="A201" s="10" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B201" s="10" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C201" s="30" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="D201" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="E201" s="9" t="s">
+      <c r="E201" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F201" s="61"/>
@@ -25751,32 +25794,32 @@
     </row>
     <row r="202">
       <c r="A202" s="10" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B202" s="10" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C202" s="62" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D202" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="E202" s="9" t="s">
-        <v>50</v>
+      <c r="E202" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F202" s="61"/>
       <c r="G202" s="61"/>
       <c r="H202" s="61"/>
       <c r="I202" s="30" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="J202" s="61"/>
       <c r="K202" s="43">
         <v>45402.0</v>
       </c>
       <c r="L202" s="43">
-        <v>45504.0</v>
+        <v>46063.0</v>
       </c>
       <c r="M202" s="30" t="s">
         <v>157</v>
@@ -25801,32 +25844,32 @@
     </row>
     <row r="203">
       <c r="A203" s="10" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C203" s="62" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D203" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="E203" s="9" t="s">
-        <v>50</v>
+      <c r="E203" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F203" s="61"/>
       <c r="G203" s="61"/>
       <c r="H203" s="61"/>
       <c r="I203" s="30" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="J203" s="61"/>
       <c r="K203" s="43">
         <v>45402.0</v>
       </c>
       <c r="L203" s="43">
-        <v>45504.0</v>
+        <v>46063.0</v>
       </c>
       <c r="M203" s="30" t="s">
         <v>157</v>
@@ -25851,28 +25894,28 @@
     </row>
     <row r="204">
       <c r="A204" s="10" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B204" s="10" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C204" s="10" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>849</v>
-      </c>
-      <c r="E204" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="E204" s="10" t="s">
         <v>50</v>
       </c>
       <c r="I204" s="10" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="K204" s="43">
         <v>45402.0</v>
       </c>
       <c r="M204" s="30" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="N204" s="10" t="s">
         <v>20</v>
@@ -25880,28 +25923,28 @@
     </row>
     <row r="205">
       <c r="A205" s="10" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B205" s="10" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D205" s="10" t="s">
-        <v>854</v>
-      </c>
-      <c r="E205" s="9" t="s">
+        <v>855</v>
+      </c>
+      <c r="E205" s="10" t="s">
         <v>50</v>
       </c>
       <c r="I205" s="10" t="s">
-        <v>287</v>
+        <v>856</v>
       </c>
       <c r="K205" s="43">
         <v>45402.0</v>
       </c>
       <c r="M205" s="30" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="N205" s="10" t="s">
         <v>20</v>
@@ -25909,29 +25952,27 @@
     </row>
     <row r="206">
       <c r="B206" s="23"/>
-      <c r="E206" s="44"/>
     </row>
     <row r="207">
       <c r="A207" s="9" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B207" s="23"/>
-      <c r="E207" s="44"/>
     </row>
     <row r="208">
       <c r="A208" s="10" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B208" s="25" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="D208" s="10" t="s">
-        <v>858</v>
-      </c>
-      <c r="E208" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="E208" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F208" s="12"/>
@@ -25970,18 +26011,18 @@
     </row>
     <row r="209">
       <c r="A209" s="10" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="D209" s="10" t="s">
-        <v>862</v>
-      </c>
-      <c r="E209" s="9" t="s">
+        <v>864</v>
+      </c>
+      <c r="E209" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F209" s="12"/>
@@ -26020,18 +26061,18 @@
     </row>
     <row r="210">
       <c r="A210" s="10" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="B210" s="11" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C210" s="10" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D210" s="10" t="s">
-        <v>866</v>
-      </c>
-      <c r="E210" s="9" t="s">
+        <v>868</v>
+      </c>
+      <c r="E210" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F210" s="12"/>
@@ -26070,18 +26111,18 @@
     </row>
     <row r="211">
       <c r="A211" s="10" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B211" s="25" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="D211" s="10" t="s">
-        <v>870</v>
-      </c>
-      <c r="E211" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="E211" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F211" s="12"/>
@@ -26120,23 +26161,23 @@
     </row>
     <row r="212">
       <c r="A212" s="10" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="B212" s="25" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="D212" s="10" t="s">
-        <v>874</v>
-      </c>
-      <c r="E212" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E212" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F212" s="12"/>
       <c r="G212" s="12" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="H212" s="12"/>
       <c r="I212" s="12"/>
@@ -26172,18 +26213,18 @@
     </row>
     <row r="213">
       <c r="A213" s="10" t="s">
+        <v>878</v>
+      </c>
+      <c r="B213" s="11" t="s">
+        <v>879</v>
+      </c>
+      <c r="C213" s="10" t="s">
+        <v>880</v>
+      </c>
+      <c r="D213" s="10" t="s">
         <v>876</v>
       </c>
-      <c r="B213" s="11" t="s">
-        <v>877</v>
-      </c>
-      <c r="C213" s="10" t="s">
-        <v>878</v>
-      </c>
-      <c r="D213" s="10" t="s">
-        <v>874</v>
-      </c>
-      <c r="E213" s="9" t="s">
+      <c r="E213" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F213" s="12"/>
@@ -26220,18 +26261,18 @@
     </row>
     <row r="214">
       <c r="A214" s="10" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B214" s="25" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="C214" s="10" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="D214" s="10" t="s">
-        <v>862</v>
-      </c>
-      <c r="E214" s="9" t="s">
+        <v>864</v>
+      </c>
+      <c r="E214" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F214" s="12"/>
@@ -26270,18 +26311,18 @@
     </row>
     <row r="215">
       <c r="A215" s="10" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B215" s="25" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="C215" s="10" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="D215" s="10" t="s">
-        <v>874</v>
-      </c>
-      <c r="E215" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="E215" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F215" s="12"/>
@@ -26320,18 +26361,18 @@
     </row>
     <row r="216">
       <c r="A216" s="10" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="B216" s="25" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C216" s="10" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="D216" s="10" t="s">
-        <v>870</v>
-      </c>
-      <c r="E216" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="E216" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F216" s="12"/>
@@ -26370,18 +26411,18 @@
     </row>
     <row r="217">
       <c r="A217" s="10" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="B217" s="25" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="D217" s="10" t="s">
-        <v>866</v>
-      </c>
-      <c r="E217" s="9" t="s">
+        <v>868</v>
+      </c>
+      <c r="E217" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F217" s="12"/>
@@ -26420,18 +26461,18 @@
     </row>
     <row r="218">
       <c r="A218" s="10" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="B218" s="11" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="D218" s="10" t="s">
-        <v>891</v>
-      </c>
-      <c r="E218" s="9" t="s">
+        <v>893</v>
+      </c>
+      <c r="E218" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F218" s="12"/>
@@ -26471,7 +26512,7 @@
       <c r="B219" s="25"/>
       <c r="C219" s="10"/>
       <c r="D219" s="10"/>
-      <c r="E219" s="9"/>
+      <c r="E219" s="10"/>
       <c r="J219" s="18"/>
       <c r="K219" s="13"/>
       <c r="M219" s="10"/>
@@ -26480,19 +26521,19 @@
     </row>
     <row r="220">
       <c r="A220" s="10" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="B220" s="25" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C220" s="10" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="D220" s="10" t="s">
-        <v>895</v>
-      </c>
-      <c r="E220" s="9" t="s">
-        <v>50</v>
+        <v>897</v>
+      </c>
+      <c r="E220" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F220" s="12"/>
       <c r="G220" s="12"/>
@@ -26505,13 +26546,13 @@
         <v>43620.0</v>
       </c>
       <c r="L220" s="13">
-        <v>45402.0</v>
+        <v>46063.0</v>
       </c>
       <c r="M220" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N220" s="10" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="O220" s="14" t="s">
         <v>208</v>
@@ -26538,10 +26579,10 @@
         <v>333</v>
       </c>
       <c r="C221" s="35" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="D221" s="35" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E221" s="35" t="s">
         <v>50</v>
@@ -26555,7 +26596,7 @@
       <c r="L221" s="37"/>
       <c r="M221" s="35"/>
       <c r="N221" s="35" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O221" s="37"/>
       <c r="P221" s="37"/>
@@ -26574,19 +26615,19 @@
     </row>
     <row r="222">
       <c r="A222" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="B222" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="C222" s="10" t="s">
+        <v>903</v>
+      </c>
+      <c r="D222" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="B222" s="10" t="s">
-        <v>900</v>
-      </c>
-      <c r="C222" s="10" t="s">
-        <v>901</v>
-      </c>
-      <c r="D222" s="10" t="s">
-        <v>898</v>
-      </c>
       <c r="E222" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F222" s="12"/>
       <c r="G222" s="12"/>
@@ -26596,12 +26637,14 @@
       <c r="K222" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L222" s="12"/>
+      <c r="L222" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M222" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N222" s="10" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O222" s="12"/>
       <c r="P222" s="12"/>
@@ -26620,19 +26663,19 @@
     </row>
     <row r="223">
       <c r="A223" s="10" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="D223" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E223" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F223" s="12"/>
       <c r="G223" s="12"/>
@@ -26642,12 +26685,14 @@
       <c r="K223" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L223" s="12"/>
+      <c r="L223" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M223" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N223" s="10" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O223" s="12"/>
       <c r="P223" s="12"/>
@@ -26666,19 +26711,19 @@
     </row>
     <row r="224">
       <c r="A224" s="10" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="B224" s="10" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="C224" s="10" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="D224" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E224" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F224" s="12"/>
       <c r="G224" s="12"/>
@@ -26688,12 +26733,14 @@
       <c r="K224" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L224" s="12"/>
+      <c r="L224" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M224" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N224" s="10" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O224" s="12"/>
       <c r="P224" s="12"/>
@@ -26712,19 +26759,19 @@
     </row>
     <row r="225">
       <c r="A225" s="10" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B225" s="10" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C225" s="10" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="D225" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E225" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F225" s="12"/>
       <c r="G225" s="12"/>
@@ -26734,12 +26781,14 @@
       <c r="K225" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L225" s="12"/>
+      <c r="L225" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M225" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N225" s="10" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O225" s="12"/>
       <c r="P225" s="12"/>
@@ -26758,19 +26807,19 @@
     </row>
     <row r="226">
       <c r="A226" s="10" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="B226" s="10" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="D226" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E226" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F226" s="12"/>
       <c r="G226" s="12"/>
@@ -26780,12 +26829,14 @@
       <c r="K226" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L226" s="12"/>
+      <c r="L226" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M226" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N226" s="10" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O226" s="12"/>
       <c r="P226" s="12"/>
@@ -26804,19 +26855,19 @@
     </row>
     <row r="227">
       <c r="A227" s="10" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B227" s="10" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C227" s="10" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="D227" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E227" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F227" s="12"/>
       <c r="G227" s="12"/>
@@ -26826,12 +26877,14 @@
       <c r="K227" s="13">
         <v>43620.0</v>
       </c>
-      <c r="L227" s="12"/>
+      <c r="L227" s="13">
+        <v>46063.0</v>
+      </c>
       <c r="M227" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N227" s="10" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="O227" s="12"/>
       <c r="P227" s="12"/>
@@ -26850,19 +26903,19 @@
     </row>
     <row r="228">
       <c r="A228" s="10" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="B228" s="25" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="D228" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E228" s="10" t="s">
-        <v>50</v>
+        <v>283</v>
       </c>
       <c r="F228" s="12"/>
       <c r="G228" s="12"/>
@@ -26875,13 +26928,13 @@
         <v>43620.0</v>
       </c>
       <c r="L228" s="13">
-        <v>45402.0</v>
+        <v>46063.0</v>
       </c>
       <c r="M228" s="10" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N228" s="10" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="O228" s="14" t="s">
         <v>208</v>
@@ -26904,13 +26957,142 @@
       <c r="B229" s="23"/>
     </row>
     <row r="230">
-      <c r="B230" s="23"/>
+      <c r="A230" s="10" t="s">
+        <v>919</v>
+      </c>
+      <c r="B230" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="C230" s="10" t="s">
+        <v>921</v>
+      </c>
+      <c r="D230" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E230" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="F230" s="12"/>
+      <c r="G230" s="12"/>
+      <c r="H230" s="12"/>
+      <c r="I230" s="12"/>
+      <c r="J230" s="12"/>
+      <c r="K230" s="13">
+        <v>46063.0</v>
+      </c>
+      <c r="L230" s="12"/>
+      <c r="M230" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N230" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O230" s="12"/>
+      <c r="P230" s="12"/>
+      <c r="Q230" s="12"/>
+      <c r="R230" s="12"/>
+      <c r="S230" s="12"/>
+      <c r="T230" s="12"/>
+      <c r="U230" s="12"/>
+      <c r="V230" s="12"/>
+      <c r="W230" s="12"/>
+      <c r="X230" s="12"/>
+      <c r="Y230" s="12"/>
+      <c r="Z230" s="12"/>
+      <c r="AA230" s="12"/>
+      <c r="AB230" s="12"/>
     </row>
     <row r="231">
-      <c r="B231" s="23"/>
+      <c r="A231" s="10" t="s">
+        <v>922</v>
+      </c>
+      <c r="B231" s="11" t="s">
+        <v>923</v>
+      </c>
+      <c r="C231" s="10" t="s">
+        <v>924</v>
+      </c>
+      <c r="D231" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E231" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="F231" s="12"/>
+      <c r="G231" s="12"/>
+      <c r="H231" s="12"/>
+      <c r="I231" s="12"/>
+      <c r="J231" s="12"/>
+      <c r="K231" s="13">
+        <v>46063.0</v>
+      </c>
+      <c r="L231" s="12"/>
+      <c r="M231" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N231" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O231" s="12"/>
+      <c r="P231" s="12"/>
+      <c r="Q231" s="12"/>
+      <c r="R231" s="12"/>
+      <c r="S231" s="12"/>
+      <c r="T231" s="12"/>
+      <c r="U231" s="12"/>
+      <c r="V231" s="12"/>
+      <c r="W231" s="12"/>
+      <c r="X231" s="12"/>
+      <c r="Y231" s="12"/>
+      <c r="Z231" s="12"/>
+      <c r="AA231" s="12"/>
+      <c r="AB231" s="12"/>
     </row>
     <row r="232">
-      <c r="B232" s="23"/>
+      <c r="A232" s="10" t="s">
+        <v>925</v>
+      </c>
+      <c r="B232" s="11" t="s">
+        <v>926</v>
+      </c>
+      <c r="C232" s="10" t="s">
+        <v>927</v>
+      </c>
+      <c r="D232" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E232" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="F232" s="12"/>
+      <c r="G232" s="12"/>
+      <c r="H232" s="12"/>
+      <c r="I232" s="12"/>
+      <c r="J232" s="12"/>
+      <c r="K232" s="13">
+        <v>46063.0</v>
+      </c>
+      <c r="L232" s="12"/>
+      <c r="M232" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N232" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O232" s="12"/>
+      <c r="P232" s="12"/>
+      <c r="Q232" s="12"/>
+      <c r="R232" s="12"/>
+      <c r="S232" s="12"/>
+      <c r="T232" s="12"/>
+      <c r="U232" s="12"/>
+      <c r="V232" s="12"/>
+      <c r="W232" s="12"/>
+      <c r="X232" s="12"/>
+      <c r="Y232" s="12"/>
+      <c r="Z232" s="12"/>
+      <c r="AA232" s="12"/>
+      <c r="AB232" s="12"/>
     </row>
     <row r="233">
       <c r="B233" s="23"/>
@@ -29780,7 +29962,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="1"/>
@@ -29798,110 +29980,110 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J4" s="18"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J7" s="18"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J8" s="18"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J9" s="18"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>917</v>
+        <v>928</v>
       </c>
       <c r="J12" s="18"/>
       <c r="K12" s="13"/>

</xml_diff>